<commit_message>
kiểm thử lần 1
</commit_message>
<xml_diff>
--- a/Kiểm Thử.xlsx
+++ b/Kiểm Thử.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="413">
   <si>
     <r>
       <rPr>
@@ -489,13 +489,13 @@
     <t>5.1</t>
   </si>
   <si>
-    <t>Kiểm tra ẩn nhân viên có chức vụ Admin với quyền quản lý</t>
+    <t>Kiểm tra cho nghỉ nhân viên có chức vụ Admin với quyền quản lý</t>
   </si>
   <si>
     <t>1. Đăng nhập tài khoản Admin hoặc Quản lý
 2. Chọn chức năng nhân viên ở màn hình chính
 3. Chọn 1 nhân viên trong danh sách
-4. Nhấn ẩn</t>
+4. Nhấn nghỉ việc</t>
   </si>
   <si>
     <t>mã nhân viên: NV001
@@ -505,7 +505,7 @@
     <t>5.2</t>
   </si>
   <si>
-    <t>Kiểm tra ẩn nhân viên có chức vụ Quản lý với quyền quản lý</t>
+    <t>Kiểm tra cho nghỉ nhân viên có chức vụ Quản lý với quyền quản lý</t>
   </si>
   <si>
     <t>mã nhân viên: NV002
@@ -515,14 +515,14 @@
     <t>5.3</t>
   </si>
   <si>
-    <t>Kiểm tra ẩn nhân viên có chức vụ thấp hơn quyền quản lý</t>
+    <t>Kiểm tra cho nghỉ nhân viên có chức vụ thấp hơn quyền quản lý</t>
   </si>
   <si>
     <t>mã nhân viên: NV004
 chức vụ: Nhân Viên Bán Hàng</t>
   </si>
   <si>
-    <t>ẩn nhân viên thành công</t>
+    <t>cho nghỉ nhân viên thành công</t>
   </si>
   <si>
     <t>6.1</t>
@@ -816,25 +816,6 @@
     <t>16.1</t>
   </si>
   <si>
-    <t>Kiểm tra ẩn loại hàng</t>
-  </si>
-  <si>
-    <t>1. Đăng nhập tài khoản Quản lý hoặc Nhân viên bán hàng hoặc Nhân viên kho
-2. Chọn chức năng sản phẩm ở màn hình chính
-3. Chọn tab thông tin loại hàng
-4. Chọn 1 loại hàng trong danh sách
-5. Nhấn ẩn</t>
-  </si>
-  <si>
-    <t>mã loại hàng: LH011</t>
-  </si>
-  <si>
-    <t>ẩn loại hàng thành công</t>
-  </si>
-  <si>
-    <t>17.1</t>
-  </si>
-  <si>
     <t>Kiểm tra hiển thị danh sách nhà cung cấp</t>
   </si>
   <si>
@@ -846,7 +827,7 @@
     <t>hiển thị danh sách nhà cung cấp</t>
   </si>
   <si>
-    <t>18.1</t>
+    <t>17.1</t>
   </si>
   <si>
     <t>Kiểm tra thêm nhà cung cấp khi để trống tên nhà cung cấp</t>
@@ -870,7 +851,7 @@
     <t>hiện thông báo chưa nhập tên nhà cung cấp</t>
   </si>
   <si>
-    <t>18.2</t>
+    <t>17.2</t>
   </si>
   <si>
     <t>Kiểm tra thêm nhà cung cấp khi để trống địa chỉ</t>
@@ -881,7 +862,7 @@
 sdt: 0914268166</t>
   </si>
   <si>
-    <t>18.3</t>
+    <t>17.3</t>
   </si>
   <si>
     <t>Kiểm tra thêm nhà cung cấp khi để trống số điện thoại</t>
@@ -892,7 +873,7 @@
 sdt:</t>
   </si>
   <si>
-    <t>18.4</t>
+    <t>17.4</t>
   </si>
   <si>
     <t>Kiểm tra thêm nhà cung cấp khi số điện thoại không phải số</t>
@@ -903,7 +884,7 @@
 sdt: abc</t>
   </si>
   <si>
-    <t>18.5</t>
+    <t>17.5</t>
   </si>
   <si>
     <t>Kiểm tra thêm nhà cung cấp khi số điện thoại không đúng định dạng</t>
@@ -914,7 +895,7 @@
 sdt: 0123456789</t>
   </si>
   <si>
-    <t>18.6</t>
+    <t>17.6</t>
   </si>
   <si>
     <t>Kiểm tra thêm nhà cung cấp khi dữ liệu hợp lệ</t>
@@ -928,26 +909,7 @@
     <t>thêm nhà cung cấp thành công</t>
   </si>
   <si>
-    <t>19.1</t>
-  </si>
-  <si>
-    <t>Kiểm tra ẩn nhà cung cấp</t>
-  </si>
-  <si>
-    <t>1. Đăng nhập tài khoản Quản lý hoặc Nhân viên kho
-2. Chọn chức năng sản phẩm ở màn hình chính
-3. Chọn tab thông tin nhà cung cấp
-4. Chọn 1 nhà cung cấp trong danh sách
-5. Nhấn ẩn</t>
-  </si>
-  <si>
-    <t>mã nhà cung cấp: CC011</t>
-  </si>
-  <si>
-    <t>ẩn nhà cung cấp thành công</t>
-  </si>
-  <si>
-    <t>20.1</t>
+    <t>18.1</t>
   </si>
   <si>
     <t>Kiểm tra hiển thị danh sách số lượng sản phẩm trong kho</t>
@@ -960,7 +922,7 @@
     <t>hiển thị danh sách số lượng sản phẩm trong kho</t>
   </si>
   <si>
-    <t>21.1</t>
+    <t>19.1</t>
   </si>
   <si>
     <t>Kiểm tra sắp xếp sản phẩm trong kho theo mã sản phẩm</t>
@@ -978,7 +940,7 @@
     <t>hiển thị danh sách sản phẩm trong kho đã được sắp xếp theo mã sản phẩm</t>
   </si>
   <si>
-    <t>21.2</t>
+    <t>19.2</t>
   </si>
   <si>
     <t>Kiểm tra sắp xếp sản phẩm trong kho theo số lượng</t>
@@ -990,7 +952,7 @@
     <t>hiển thị danh sách sản phẩm trong kho đã được sắp xếp theo số lượng</t>
   </si>
   <si>
-    <t>22.1</t>
+    <t>20.1</t>
   </si>
   <si>
     <t>Kiểm tra hiển thị danh sách khách hàng</t>
@@ -1003,7 +965,7 @@
     <t>hiển thị danh sách khách hàng</t>
   </si>
   <si>
-    <t>23.1</t>
+    <t>21.1</t>
   </si>
   <si>
     <t>Kiểm tra thêm khách hàng khi để trống họ tên</t>
@@ -1021,7 +983,7 @@
 sdt: 0914268166</t>
   </si>
   <si>
-    <t>23.2</t>
+    <t>21.2</t>
   </si>
   <si>
     <t>Kiểm tra thêm khách hàng khi họ tên không đúng định dạng</t>
@@ -1031,7 +993,7 @@
 sdt: 0914268166</t>
   </si>
   <si>
-    <t>23.3</t>
+    <t>21.3</t>
   </si>
   <si>
     <t>Kiểm tra thêm khách hàng khi để trống số điện thoại</t>
@@ -1041,7 +1003,7 @@
 sdt:</t>
   </si>
   <si>
-    <t>23.4</t>
+    <t>21.4</t>
   </si>
   <si>
     <t>Kiểm tra thêm khách hàng khi số điện thoại không phải số</t>
@@ -1051,7 +1013,7 @@
 sdt: abc</t>
   </si>
   <si>
-    <t>23.5</t>
+    <t>21.5</t>
   </si>
   <si>
     <t>Kiểm tra thêm khách hàng khi số điện thoại không đúng định dạng</t>
@@ -1061,7 +1023,7 @@
 sdt: 0123456789</t>
   </si>
   <si>
-    <t>23.6</t>
+    <t>21.6</t>
   </si>
   <si>
     <t>Kiểm tra thêm khách hàng khi dữ liệu hợp lệ</t>
@@ -1074,25 +1036,7 @@
     <t>thêm khách hàng thành công</t>
   </si>
   <si>
-    <t>24.1</t>
-  </si>
-  <si>
-    <t>Kiểm tra ẩn khách hàng</t>
-  </si>
-  <si>
-    <t>1. Đăng nhập tài khoản Quản lý hoặc Nhân viên bán hàng
-2. Chọn chức năng khách hàng ở màn hình chính
-3. Chọn 1 khách hàng trong danh sách
-4. Nhấn ẩn</t>
-  </si>
-  <si>
-    <t>mã khách hàng: KH011</t>
-  </si>
-  <si>
-    <t>ẩn khách hàng thành công</t>
-  </si>
-  <si>
-    <t>25.1</t>
+    <t>22.1</t>
   </si>
   <si>
     <t>Kiểm tra sắp xếp khách hàng theo mã khách hàng</t>
@@ -1110,7 +1054,7 @@
     <t>hiển thị danh sách khách hàng đã được sắp xếp theo mã</t>
   </si>
   <si>
-    <t>25.2</t>
+    <t>22.2</t>
   </si>
   <si>
     <t>Kiểm tra sắp xếp khách hàng theo tên khách hàng</t>
@@ -1122,7 +1066,7 @@
     <t>hiển thị danh sách khách hàng đã được sắp xếp theo tên khách hàng</t>
   </si>
   <si>
-    <t>26.1</t>
+    <t>23.1</t>
   </si>
   <si>
     <t>Kiểm tra hiển thị danh sách phiếu nhập</t>
@@ -1135,7 +1079,7 @@
     <t>hiển thị danh sách phiếu nhập</t>
   </si>
   <si>
-    <t>27.1</t>
+    <t>24.1</t>
   </si>
   <si>
     <t>Kiểm tra thêm phiếu nhập khi dữ liệu hợp lệ</t>
@@ -1154,25 +1098,7 @@
     <t>thêm phiếu nhập thành công</t>
   </si>
   <si>
-    <t>28.1</t>
-  </si>
-  <si>
-    <t>Kiểm tra ẩn phiếu nhập</t>
-  </si>
-  <si>
-    <t>1. Đăng nhập tài khoản Quản lý hoặc Nhân viên kho
-2. Chọn chức năng nhập hàng ở màn hình chính
-3. Chọn 1 phiếu nhập trong danh sách
-4. Nhấn ẩn</t>
-  </si>
-  <si>
-    <t>mã phiếu nhập: PN011</t>
-  </si>
-  <si>
-    <t>ẩn phiếu nhập thành công</t>
-  </si>
-  <si>
-    <t>29.1</t>
+    <t>25.1</t>
   </si>
   <si>
     <t>Kiểm tra hiển thị chi tiết phiếu nhập</t>
@@ -1189,7 +1115,7 @@
     <t>hiển thị chi tiết phiếu nhập</t>
   </si>
   <si>
-    <t>30.1</t>
+    <t>26.1</t>
   </si>
   <si>
     <t>Kiểm tra thêm chi tiết phiếu nhập của nhân viên khác</t>
@@ -1204,7 +1130,7 @@
     <t>hiện thông báo không thể thêm chi tiết cho phiếu nhập của nhân viên khác</t>
   </si>
   <si>
-    <t>30.2</t>
+    <t>26.2</t>
   </si>
   <si>
     <t>Kiểm tra thêm chi tiết phiếu nhập khi để trống tên sản phẩm</t>
@@ -1234,7 +1160,7 @@
     <t>hiện thông báo chưa nhập tên sản phẩm</t>
   </si>
   <si>
-    <t>30.3</t>
+    <t>26.3</t>
   </si>
   <si>
     <t>Kiểm tra thêm chi tiết phiếu nhập khi tên sản phẩm đã tồn tại</t>
@@ -1251,7 +1177,7 @@
     <t>hiện thông báo tên sản phẩm đã tồn tại</t>
   </si>
   <si>
-    <t>30.4</t>
+    <t>26.4</t>
   </si>
   <si>
     <t>Kiểm tra thêm chi tiết phiếu nhập khi để trống số lượng</t>
@@ -1268,7 +1194,7 @@
     <t>hiện thông báo chưa nhập số lượng</t>
   </si>
   <si>
-    <t>30.5</t>
+    <t>26.5</t>
   </si>
   <si>
     <t>Kiểm tra thêm chi tiết phiếu nhập khi số lượng không phải số</t>
@@ -1285,7 +1211,7 @@
     <t>hiện thông báo số lượng phải là số</t>
   </si>
   <si>
-    <t>30.6</t>
+    <t>26.6</t>
   </si>
   <si>
     <t>Kiểm tra thêm chi tiết phiếu nhập khi để trống giá nhập</t>
@@ -1302,7 +1228,7 @@
     <t>hiện thông báo chưa nhập giá nhập</t>
   </si>
   <si>
-    <t>30.7</t>
+    <t>26.7</t>
   </si>
   <si>
     <t>Kiểm tra thêm chi tiết phiếu nhập khi giá nhập không phải số</t>
@@ -1319,7 +1245,7 @@
     <t>hiện thông báo giá nhập phải là số</t>
   </si>
   <si>
-    <t>30.8</t>
+    <t>26.8</t>
   </si>
   <si>
     <t>Kiểm tra thêm chi tiết phiếu nhập khi giá nhập dưới 1000</t>
@@ -1336,7 +1262,7 @@
     <t>hiện thông báo giá nhập phải lớn hơn 1000</t>
   </si>
   <si>
-    <t>30.9</t>
+    <t>26.9</t>
   </si>
   <si>
     <t>Kiểm tra thêm chi tiết phiếu nhập khi để trống ngày sản xuất</t>
@@ -1353,7 +1279,7 @@
     <t>hiện thông báo chưa chọn ngày sản xuất</t>
   </si>
   <si>
-    <t>30.10</t>
+    <t>26.10</t>
   </si>
   <si>
     <t>Kiểm tra thêm chi tiết phiếu nhập khi để trống hạn sử dụng</t>
@@ -1370,7 +1296,7 @@
     <t>hiện thông báo chưa chọn hạn sử dụng</t>
   </si>
   <si>
-    <t>30.11</t>
+    <t>26.11</t>
   </si>
   <si>
     <t>Kiểm tra thêm chi tiết phiếu nhập khi ngày sản xuất lớn hơn hạn sử dụng</t>
@@ -1387,7 +1313,7 @@
     <t>hiện thông báo ngày sản xuất không lớn hơn ngày sử dụng</t>
   </si>
   <si>
-    <t>30.12</t>
+    <t>26.12</t>
   </si>
   <si>
     <t>Kiểm tra thêm chi tiết phiếu nhập khi dữ liệu hợp lệ</t>
@@ -1404,24 +1330,7 @@
     <t>thêm chi tiết phiếu nhập thành công</t>
   </si>
   <si>
-    <t>31.1</t>
-  </si>
-  <si>
-    <t>Kiểm tra ẩn chi tiết phiếu nhập</t>
-  </si>
-  <si>
-    <t>1. Đăng nhập tài khoản Quản lý hoặc Nhân viên kho
-2. Chọn chức năng nhập hàng ở màn hình chính
-3. Chọn 1 phiếu nhập trong danh sách
-4. Chọn 1 chi tiết phiếu nhập
-5. Nhấn ẩn</t>
-  </si>
-  <si>
-    <t>mã phiếu nhập: PN011
-mã sản phẩm: SP001</t>
-  </si>
-  <si>
-    <t>38.1</t>
+    <t>33.1</t>
   </si>
   <si>
     <t>Kiểm tra chức năng hiển thị danh sách phiếu nhập và hóa đơn</t>
@@ -1434,7 +1343,7 @@
     <t>hiển thị danh sách phiếu nhập và danh sách hóa đơn</t>
   </si>
   <si>
-    <t>39.1</t>
+    <t>34.1</t>
   </si>
   <si>
     <t>Kiểm tra thống kê khi chọn ngày thống kê không hợp lệ</t>
@@ -1454,7 +1363,7 @@
     <t>hiện thông báo ngày thống kê không hợp lệ</t>
   </si>
   <si>
-    <t>39.2</t>
+    <t>34.2</t>
   </si>
   <si>
     <t>Kiểm tra thống kê khi dữ liệu hợp lệ</t>
@@ -1467,7 +1376,7 @@
     <t>hiển thị biểu đồ sau khi thống kê</t>
   </si>
   <si>
-    <t>40.1</t>
+    <t>35.1</t>
   </si>
   <si>
     <t>1. Kiểm tra in thống kê</t>
@@ -1556,12 +1465,12 @@
 15. Kiểm tra thêm nhân viên khi dữ liệu hợp lệ</t>
   </si>
   <si>
-    <t>Kiểm tra chức năng ẩn nhân viên</t>
-  </si>
-  <si>
-    <t>1. Kiểm tra ẩn nhân viên có chức vụ Admin với quyền quản lý
-2. Kiểm tra ẩn nhân viên có chức vụ Quản lý với quyền quản lý 
-3. Kiểm tra ẩn nhân viên có chức vụ thấp hơn quyền quản lý</t>
+    <t>Kiểm tra chức năng cho nghỉ nhân viên</t>
+  </si>
+  <si>
+    <t>1. Kiểm tra cho nghỉ nhân viên có chức vụ Admin với quyền quản lý
+2. Kiểm tra cho nghỉ nhân viên có chức vụ Quản lý với quyền quản lý 
+3. Kiểm tra cho nghỉ nhân viên có chức vụ thấp hơn quyền quản lý</t>
   </si>
   <si>
     <t>Kiểm tra chức năng sắp xếp nhân viên</t>
@@ -1591,8 +1500,8 @@
     <t>Kiểm tra chức năng ẩn tài khoản</t>
   </si>
   <si>
-    <t>1. Kiểm tra ẩn tài khoản khi nhân viên chưa được ẩn
-2. Kiểm tra ẩn tài khoản với nhân viên đã được ẩn</t>
+    <t>1. Kiểm tra ẩn tài khoản khi nhân viên chưa nghỉ
+2. Kiểm tra ẩn tài khoản với nhân viên đã nghỉ</t>
   </si>
   <si>
     <t>Kiểm tra chức năng sắp xếp tài khoản</t>
@@ -1632,12 +1541,6 @@
   <si>
     <t>1. Kiểm tra thêm loại hàng khi để trống tên loại hàng
 2. Kiểm tra thêm loại hàng khi dữ liệu hợp lệ</t>
-  </si>
-  <si>
-    <t>Kiểm tra chức năng ẩn loại hàng</t>
-  </si>
-  <si>
-    <t>1. Kiểm tra ẩn loại hàng</t>
   </si>
   <si>
     <t>Kiểm tra chức năng hiển thị danh sách nhà cung cấp</t>
@@ -1657,12 +1560,6 @@
 6. Kiểm tra thêm nhà cung cấp khi dữ liệu hợp lệ</t>
   </si>
   <si>
-    <t>Kiểm tra chức năng ẩn nhà cung cấp</t>
-  </si>
-  <si>
-    <t>1. Kiểm tra ẩn nhà cung cấp</t>
-  </si>
-  <si>
     <t>Kiểm tra chức năng hiển thị danh sách số lượng sản phẩm trong kho</t>
   </si>
   <si>
@@ -1693,12 +1590,6 @@
 5. Kiểm tra thêm khách hàng khi dữ liệu hợp lệ</t>
   </si>
   <si>
-    <t>Kiểm tra chức năng ẩn khách hàng</t>
-  </si>
-  <si>
-    <t>1. Kiểm tra ẩn khách hàng</t>
-  </si>
-  <si>
     <t>Kiểm tra chức năng sắp xếp khách hàng</t>
   </si>
   <si>
@@ -1716,12 +1607,6 @@
   </si>
   <si>
     <t>1. Kiểm tra thêm phiếu nhập khi dữ liệu hợp lệ</t>
-  </si>
-  <si>
-    <t>Kiểm tra chức năng ẩn phiếu nhập</t>
-  </si>
-  <si>
-    <t>1. Kiểm tra ẩn phiếu nhập</t>
   </si>
   <si>
     <t>Kiểm tra chức năng hiển thị chi tiết phiếu nhập</t>
@@ -1745,12 +1630,6 @@
 10. Kiểm tra thêm chi tiết phiếu nhập khi để trống hạn sử dụng
 11. Kiểm tra thêm chi tiết phiếu nhập khi ngày sản xuất lớn hơn hạn sử dụng
 12. Kiểm tra thêm chi tiết phiếu nhập khi dữ liệu hợp lệ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kiểm tra chức năng ẩn chi tiết phiếu </t>
-  </si>
-  <si>
-    <t>1. Kiểm tra ẩn chi tiết phiếu nhập</t>
   </si>
   <si>
     <t>Kiểm tra chức năng thêm hóa đơn</t>
@@ -3011,10 +2890,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:H91"/>
+  <dimension ref="B1:H86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="E91" sqref="E91"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -4071,7 +3950,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" ht="158.4" spans="2:8">
+    <row r="48" ht="100.8" spans="2:8">
       <c r="B48" s="3" t="s">
         <v>191</v>
       </c>
@@ -4081,27 +3960,27 @@
       <c r="D48" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="F48" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="G48" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" ht="187.2" spans="2:8">
+      <c r="B49" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="G48" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="49" ht="100.8" spans="2:8">
-      <c r="B49" s="3" t="s">
+      <c r="C49" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="D49" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="E49" s="3" t="s">
         <v>198</v>
       </c>
       <c r="F49" s="3" t="s">
@@ -4122,16 +4001,16 @@
         <v>201</v>
       </c>
       <c r="D50" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="E50" s="3" t="s">
-        <v>203</v>
-      </c>
       <c r="F50" s="3" t="s">
-        <v>204</v>
+        <v>91</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>204</v>
+        <v>91</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>12</v>
@@ -4139,22 +4018,22 @@
     </row>
     <row r="51" ht="187.2" spans="2:8">
       <c r="B51" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>207</v>
-      </c>
       <c r="F51" s="3" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>12</v>
@@ -4162,22 +4041,22 @@
     </row>
     <row r="52" ht="187.2" spans="2:8">
       <c r="B52" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>210</v>
-      </c>
       <c r="F52" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>12</v>
@@ -4185,22 +4064,22 @@
     </row>
     <row r="53" ht="187.2" spans="2:8">
       <c r="B53" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E53" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>213</v>
-      </c>
       <c r="F53" s="3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="H53" s="3" t="s">
         <v>12</v>
@@ -4208,154 +4087,154 @@
     </row>
     <row r="54" ht="187.2" spans="2:8">
       <c r="B54" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E54" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="F54" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="E54" s="3" t="s">
+      <c r="G54" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" ht="72" spans="2:8">
+      <c r="B55" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="F54" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H54" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="55" ht="187.2" spans="2:8">
-      <c r="B55" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="D55" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="E55" s="3" t="s">
+      <c r="F55" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="G55" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" ht="100.8" spans="2:8">
+      <c r="B56" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="G55" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="H55" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="56" ht="144" spans="2:8">
-      <c r="B56" s="3" t="s">
+      <c r="C56" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="D56" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="E56" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="F56" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="F56" s="3" t="s">
+      <c r="G56" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" ht="100.8" spans="2:8">
+      <c r="B57" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="G56" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="H56" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="57" ht="72" spans="2:8">
-      <c r="B57" s="3" t="s">
+      <c r="C57" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="D57" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="E57" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="F57" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="F57" s="3" t="s">
+      <c r="G57" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" ht="86.4" spans="2:8">
+      <c r="B58" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="G57" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="58" ht="100.8" spans="2:8">
-      <c r="B58" s="3" t="s">
+      <c r="C58" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="D58" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="F58" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="G58" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" ht="144" spans="2:8">
+      <c r="B59" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="F58" s="3" t="s">
+      <c r="C59" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="G58" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="H58" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="59" ht="100.8" spans="2:8">
-      <c r="B59" s="3" t="s">
+      <c r="D59" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="E59" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="E59" s="3" t="s">
+      <c r="F59" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="60" ht="144" spans="2:8">
+      <c r="B60" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="F59" s="3" t="s">
+      <c r="C60" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="G59" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="H59" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="60" ht="86.4" spans="2:8">
-      <c r="B60" s="3" t="s">
+      <c r="D60" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E60" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>241</v>
-      </c>
       <c r="F60" s="3" t="s">
-        <v>242</v>
+        <v>45</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>242</v>
+        <v>45</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>12</v>
@@ -4363,22 +4242,22 @@
     </row>
     <row r="61" ht="144" spans="2:8">
       <c r="B61" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="H61" s="3" t="s">
         <v>12</v>
@@ -4386,22 +4265,22 @@
     </row>
     <row r="62" ht="144" spans="2:8">
       <c r="B62" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D62" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E62" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="E62" s="3" t="s">
-        <v>249</v>
-      </c>
       <c r="F62" s="3" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="H62" s="3" t="s">
         <v>12</v>
@@ -4409,22 +4288,22 @@
     </row>
     <row r="63" ht="144" spans="2:8">
       <c r="B63" s="3" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="H63" s="3" t="s">
         <v>12</v>
@@ -4432,91 +4311,88 @@
     </row>
     <row r="64" ht="144" spans="2:8">
       <c r="B64" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65" ht="115.2" spans="2:8">
+      <c r="B65" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C65" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="D64" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="E64" s="3" t="s">
+      <c r="D65" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="F64" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G64" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H64" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="65" ht="144" spans="2:8">
-      <c r="B65" s="3" t="s">
+      <c r="E65" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="F65" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="D65" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="E65" s="3" t="s">
+      <c r="G65" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" ht="115.2" spans="2:8">
+      <c r="B66" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="F65" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H65" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="66" ht="144" spans="2:8">
-      <c r="B66" s="3" t="s">
+      <c r="C66" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="D66" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="E66" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="D66" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="E66" s="3" t="s">
+      <c r="F66" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="F66" s="3" t="s">
+      <c r="G66" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" ht="72" spans="2:8">
+      <c r="B67" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="G66" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="H66" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="67" ht="129.6" spans="2:8">
-      <c r="B67" s="3" t="s">
+      <c r="C67" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="D67" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="F67" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="E67" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>267</v>
-      </c>
       <c r="G67" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H67" s="3" t="s">
         <v>12</v>
@@ -4524,157 +4400,160 @@
     </row>
     <row r="68" ht="115.2" spans="2:8">
       <c r="B68" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D68" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="E68" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="F68" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="G68" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" ht="100.8" spans="2:8">
+      <c r="B69" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="F68" s="3" t="s">
+      <c r="C69" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="G68" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="H68" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="69" ht="115.2" spans="2:8">
-      <c r="B69" s="3" t="s">
+      <c r="D69" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="E69" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="D69" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="E69" s="3" t="s">
+      <c r="F69" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="F69" s="3" t="s">
+      <c r="G69" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="H69" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" ht="115.2" spans="2:8">
+      <c r="B70" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="G69" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="H69" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="70" ht="72" spans="2:8">
-      <c r="B70" s="3" t="s">
+      <c r="C70" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="D70" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="E70" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="F70" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="F70" s="3" t="s">
+      <c r="G70" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="71" ht="216" spans="2:8">
+      <c r="B71" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="G70" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="H70" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="71" ht="115.2" spans="2:8">
-      <c r="B71" s="3" t="s">
+      <c r="C71" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="D71" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="E71" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="E71" s="3" t="s">
+      <c r="F71" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="F71" s="3" t="s">
+      <c r="G71" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72" ht="216" spans="2:8">
+      <c r="B72" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="G71" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="H71" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="72" ht="115.2" spans="2:8">
-      <c r="B72" s="3" t="s">
+      <c r="C72" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="D72" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="E72" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="F72" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="E72" s="3" t="s">
+      <c r="G72" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="H72" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" ht="216" spans="2:8">
+      <c r="B73" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="F72" s="3" t="s">
+      <c r="C73" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="G72" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="H72" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="73" ht="100.8" spans="2:8">
-      <c r="B73" s="3" t="s">
+      <c r="D73" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="E73" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="F73" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="G73" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="H73" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" ht="216" spans="2:8">
+      <c r="B74" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="E73" s="3" t="s">
+      <c r="C74" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="F73" s="3" t="s">
+      <c r="D74" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="E74" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="G73" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="H73" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="74" ht="115.2" spans="2:8">
-      <c r="B74" s="3" t="s">
+      <c r="F74" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="C74" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="F74" s="3" t="s">
-        <v>299</v>
-      </c>
       <c r="G74" s="3" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H74" s="3" t="s">
         <v>12</v>
@@ -4682,22 +4561,22 @@
     </row>
     <row r="75" ht="216" spans="2:8">
       <c r="B75" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F75" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="C75" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="E75" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F75" s="3" t="s">
-        <v>304</v>
-      </c>
       <c r="G75" s="3" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="H75" s="3" t="s">
         <v>12</v>
@@ -4705,22 +4584,22 @@
     </row>
     <row r="76" ht="216" spans="2:8">
       <c r="B76" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="H76" s="3" t="s">
         <v>12</v>
@@ -4728,22 +4607,22 @@
     </row>
     <row r="77" ht="216" spans="2:8">
       <c r="B77" s="3" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="H77" s="3" t="s">
         <v>12</v>
@@ -4751,22 +4630,22 @@
     </row>
     <row r="78" ht="216" spans="2:8">
       <c r="B78" s="3" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="H78" s="3" t="s">
         <v>12</v>
@@ -4774,22 +4653,22 @@
     </row>
     <row r="79" ht="216" spans="2:8">
       <c r="B79" s="3" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="H79" s="3" t="s">
         <v>12</v>
@@ -4797,22 +4676,22 @@
     </row>
     <row r="80" ht="216" spans="2:8">
       <c r="B80" s="3" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="H80" s="3" t="s">
         <v>12</v>
@@ -4820,228 +4699,113 @@
     </row>
     <row r="81" ht="216" spans="2:8">
       <c r="B81" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="83" ht="72" spans="2:8">
+      <c r="B83" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="C83" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="D81" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="E81" s="3" t="s">
+      <c r="D83" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="F81" s="3" t="s">
+      <c r="F83" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="G81" s="3" t="s">
+      <c r="G83" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="H81" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="82" ht="216" spans="2:8">
-      <c r="B82" s="3" t="s">
+      <c r="H83" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="84" ht="144" spans="2:8">
+      <c r="B84" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="C82" s="3" t="s">
+      <c r="C84" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="D82" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="E82" s="3" t="s">
+      <c r="D84" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="F82" s="3" t="s">
+      <c r="E84" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="G82" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="H82" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="83" ht="216" spans="2:8">
-      <c r="B83" s="3" t="s">
+      <c r="F84" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="G84" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" ht="144" spans="2:8">
+      <c r="B85" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="D83" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="E83" s="3" t="s">
+      <c r="C85" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="F83" s="3" t="s">
+      <c r="D85" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="E85" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="G83" s="3" t="s">
-        <v>336</v>
-      </c>
-      <c r="H83" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="84" ht="216" spans="2:8">
-      <c r="B84" s="3" t="s">
+      <c r="F85" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="C84" s="3" t="s">
+      <c r="G85" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="H85" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86" ht="187.2" spans="2:8">
+      <c r="B86" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="D84" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="E84" s="3" t="s">
+      <c r="C86" t="s">
         <v>339</v>
       </c>
-      <c r="F84" s="3" t="s">
+      <c r="D86" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="G84" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="H84" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="85" ht="216" spans="2:8">
-      <c r="B85" s="3" t="s">
+      <c r="E86" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="F86" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="D85" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="F85" s="3" t="s">
-        <v>344</v>
-      </c>
-      <c r="G85" s="3" t="s">
-        <v>344</v>
-      </c>
-      <c r="H85" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="86" ht="144" spans="2:8">
-      <c r="B86" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>290</v>
-      </c>
       <c r="G86" s="3" t="s">
-        <v>290</v>
+        <v>342</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="88" ht="72" spans="2:8">
-      <c r="B88" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="F88" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="G88" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="H88" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="89" ht="144" spans="2:8">
-      <c r="B89" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>356</v>
-      </c>
-      <c r="F89" s="3" t="s">
-        <v>357</v>
-      </c>
-      <c r="G89" s="3" t="s">
-        <v>357</v>
-      </c>
-      <c r="H89" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="90" ht="144" spans="2:8">
-      <c r="B90" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="F90" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="G90" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="H90" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="91" ht="187.2" spans="2:8">
-      <c r="B91" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="C91" t="s">
-        <v>363</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>366</v>
-      </c>
-      <c r="G91" s="3" t="s">
-        <v>366</v>
-      </c>
-      <c r="H91" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -5054,10 +4818,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:D42"/>
+  <dimension ref="B1:D37"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -5073,10 +4837,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>367</v>
+        <v>343</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>368</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3" ht="72" spans="2:4">
@@ -5084,10 +4848,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>369</v>
+        <v>345</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>370</v>
+        <v>346</v>
       </c>
     </row>
     <row r="4" spans="2:4">
@@ -5095,10 +4859,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="D4" t="s">
-        <v>372</v>
+        <v>348</v>
       </c>
     </row>
     <row r="5" spans="2:4">
@@ -5106,10 +4870,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>373</v>
+        <v>349</v>
       </c>
       <c r="D5" t="s">
-        <v>374</v>
+        <v>350</v>
       </c>
     </row>
     <row r="6" ht="216" spans="2:4">
@@ -5117,10 +4881,10 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>375</v>
+        <v>351</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>376</v>
+        <v>352</v>
       </c>
     </row>
     <row r="7" ht="43.2" spans="2:4">
@@ -5128,10 +4892,10 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>377</v>
+        <v>353</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>378</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8" ht="28.8" spans="2:4">
@@ -5139,10 +4903,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>379</v>
+        <v>355</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>380</v>
+        <v>356</v>
       </c>
     </row>
     <row r="9" spans="2:4">
@@ -5150,10 +4914,10 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>381</v>
+        <v>357</v>
       </c>
       <c r="D9" t="s">
-        <v>382</v>
+        <v>358</v>
       </c>
     </row>
     <row r="10" ht="86.4" spans="2:4">
@@ -5161,10 +4925,10 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>383</v>
+        <v>359</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>384</v>
+        <v>360</v>
       </c>
     </row>
     <row r="11" ht="28.8" spans="2:4">
@@ -5172,10 +4936,10 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>385</v>
+        <v>361</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>386</v>
+        <v>362</v>
       </c>
     </row>
     <row r="12" ht="28.8" spans="2:4">
@@ -5183,10 +4947,10 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>387</v>
+        <v>363</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>388</v>
+        <v>364</v>
       </c>
     </row>
     <row r="13" spans="2:4">
@@ -5194,10 +4958,10 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>389</v>
+        <v>365</v>
       </c>
       <c r="D13" t="s">
-        <v>390</v>
+        <v>366</v>
       </c>
     </row>
     <row r="14" ht="28.8" spans="2:4">
@@ -5205,10 +4969,10 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>391</v>
+        <v>367</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>392</v>
+        <v>368</v>
       </c>
     </row>
     <row r="15" spans="2:4">
@@ -5216,10 +4980,10 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>393</v>
+        <v>369</v>
       </c>
       <c r="D15" t="s">
-        <v>394</v>
+        <v>370</v>
       </c>
     </row>
     <row r="16" spans="2:4">
@@ -5227,10 +4991,10 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>395</v>
+        <v>371</v>
       </c>
       <c r="D16" t="s">
-        <v>396</v>
+        <v>372</v>
       </c>
     </row>
     <row r="17" ht="28.8" spans="2:4">
@@ -5238,10 +5002,10 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>397</v>
+        <v>373</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>398</v>
+        <v>374</v>
       </c>
     </row>
     <row r="18" spans="2:4">
@@ -5249,43 +5013,43 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>399</v>
+        <v>375</v>
       </c>
       <c r="D18" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="19" ht="86.4" spans="2:4">
       <c r="B19">
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>401</v>
-      </c>
-      <c r="D19" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="20" ht="86.4" spans="2:4">
+        <v>377</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
       <c r="B20">
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>403</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4">
+        <v>379</v>
+      </c>
+      <c r="D20" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="21" ht="28.8" spans="2:4">
       <c r="B21">
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>405</v>
-      </c>
-      <c r="D21" t="s">
-        <v>406</v>
+        <v>381</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="22" spans="2:4">
@@ -5293,43 +5057,43 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>407</v>
+        <v>383</v>
       </c>
       <c r="D22" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="23" ht="28.8" spans="2:4">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="23" ht="86.4" spans="2:4">
       <c r="B23">
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>409</v>
+        <v>385</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="24" ht="28.8" spans="2:4">
       <c r="B24">
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>411</v>
-      </c>
-      <c r="D24" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="25" ht="86.4" spans="2:4">
+        <v>387</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
       <c r="B25">
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>413</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>414</v>
+        <v>389</v>
+      </c>
+      <c r="D25" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="26" spans="2:4">
@@ -5337,54 +5101,54 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>415</v>
+        <v>391</v>
       </c>
       <c r="D26" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="27" ht="28.8" spans="2:4">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
       <c r="B27">
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>417</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4">
+        <v>393</v>
+      </c>
+      <c r="D27" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="28" ht="172.8" spans="2:4">
       <c r="B28">
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>419</v>
-      </c>
-      <c r="D28" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4">
+        <v>395</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="29" ht="43.2" spans="2:4">
       <c r="B29">
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>421</v>
-      </c>
-      <c r="D29" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4">
+        <v>397</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="30" ht="28.8" spans="2:4">
       <c r="B30">
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>423</v>
-      </c>
-      <c r="D30" t="s">
-        <v>424</v>
+        <v>399</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="31" spans="2:4">
@@ -5392,21 +5156,21 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>425</v>
+        <v>401</v>
       </c>
       <c r="D31" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="32" ht="172.8" spans="2:4">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="32" ht="28.8" spans="2:4">
       <c r="B32">
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>427</v>
+        <v>403</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>428</v>
+        <v>404</v>
       </c>
     </row>
     <row r="33" spans="2:4">
@@ -5414,109 +5178,54 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>429</v>
+        <v>405</v>
       </c>
       <c r="D33" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="34" ht="43.2" spans="2:4">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
       <c r="B34">
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>431</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="35" ht="28.8" spans="2:4">
+        <v>407</v>
+      </c>
+      <c r="D34" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
       <c r="B35">
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>433</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4">
+        <v>326</v>
+      </c>
+      <c r="D35" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="36" ht="28.8" spans="2:4">
       <c r="B36">
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>435</v>
-      </c>
-      <c r="D36" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="37" ht="28.8" spans="2:4">
+        <v>410</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4">
       <c r="B37">
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>437</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4">
-      <c r="B38">
-        <v>36</v>
-      </c>
-      <c r="C38" t="s">
-        <v>439</v>
-      </c>
-      <c r="D38" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4">
-      <c r="B39">
-        <v>37</v>
-      </c>
-      <c r="C39" t="s">
-        <v>441</v>
-      </c>
-      <c r="D39" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4">
-      <c r="B40">
-        <v>38</v>
-      </c>
-      <c r="C40" t="s">
-        <v>350</v>
-      </c>
-      <c r="D40" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="41" ht="28.8" spans="2:4">
-      <c r="B41">
-        <v>39</v>
-      </c>
-      <c r="C41" t="s">
-        <v>444</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4">
-      <c r="B42">
-        <v>40</v>
-      </c>
-      <c r="C42" t="s">
-        <v>446</v>
-      </c>
-      <c r="D42" t="s">
-        <v>363</v>
+        <v>412</v>
+      </c>
+      <c r="D37" t="s">
+        <v>339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
kiểm thử lần 2
</commit_message>
<xml_diff>
--- a/Kiểm Thử.xlsx
+++ b/Kiểm Thử.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="473">
   <si>
     <r>
       <rPr>
@@ -647,7 +647,7 @@
     <t>9.1</t>
   </si>
   <si>
-    <t>Kiểm tra ẩn tài khoản khi nhân viên chưa được ẩn</t>
+    <t>Kiểm tra ẩn tài khoản khi nhân viên còn làm việc</t>
   </si>
   <si>
     <t>1. Đăng nhập tài khoản Admin
@@ -666,7 +666,7 @@
     <t>9.2</t>
   </si>
   <si>
-    <t>Kiểm tra ẩn tài khoản với nhân viên đã được ẩn</t>
+    <t>Kiểm tra ẩn tài khoản với nhân viên đã nghỉ việc</t>
   </si>
   <si>
     <t>mã nhân viên: NV012</t>
@@ -1316,6 +1316,23 @@
     <t>26.12</t>
   </si>
   <si>
+    <t>Kiểm tra thêm chi tiết phiếu nhập khi hạn sử dụng bé hơn ngày hiện tại</t>
+  </si>
+  <si>
+    <t>tên sản phẩm: coca
+loại hàng: đồ uống
+số lượng: 50
+giá nhập: 8000
+ngày sản xuất: 01/02/2023
+hạn sử dụng: 02/03/2023</t>
+  </si>
+  <si>
+    <t>hiện thông báo hạn sử dụng phải lớn hơn hiện tại</t>
+  </si>
+  <si>
+    <t>26.13</t>
+  </si>
+  <si>
     <t>Kiểm tra thêm chi tiết phiếu nhập khi dữ liệu hợp lệ</t>
   </si>
   <si>
@@ -1330,7 +1347,260 @@
     <t>thêm chi tiết phiếu nhập thành công</t>
   </si>
   <si>
-    <t>33.1</t>
+    <t>27.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kiểm tra thêm hóa đơn khi chưa nhập tên khách hàng</t>
+  </si>
+  <si>
+    <t>1. Đăng nhập tài khoản Quản lý hoặc Nhân viên bán hàng
+2. Chọn chức năng bán hàng ở màn hình chính
+3. Nhấn hóa đơn
+4. Nhập tên khách hàng hàng
+5. Nhấn Enter trên bàn phím
+6. Chọn ngày
+7. Nhấn lưu</t>
+  </si>
+  <si>
+    <t>tên khách hàng:
+ngày: 01/11/2023</t>
+  </si>
+  <si>
+    <t>hiện thông báo chưa nhập tên khách hàng</t>
+  </si>
+  <si>
+    <t>27.2</t>
+  </si>
+  <si>
+    <t>Kiểm tra thêm hóa đơn khi khách hàng chưa tồn tại</t>
+  </si>
+  <si>
+    <t>tên khách hàng: nhân
+ngày: 01/11/2023</t>
+  </si>
+  <si>
+    <t>hiện thông báo khách hàng chưa tồn tại và hiện nút thêm khách hàng</t>
+  </si>
+  <si>
+    <t>27.3</t>
+  </si>
+  <si>
+    <t>Kiểm tra thêm hóa đơn khi chưa chọn ngày</t>
+  </si>
+  <si>
+    <t>tên khách hàng: Hoàng Hảo
+ngày:</t>
+  </si>
+  <si>
+    <t>hiện thông báo chưa chọn ngày</t>
+  </si>
+  <si>
+    <t>27.4</t>
+  </si>
+  <si>
+    <t>Kiểm tra thêm hóa đơn khi dữ liệu hợp lệ</t>
+  </si>
+  <si>
+    <t>tên khách hàng: Hoàng Hảo
+ngày: 01/11/2023</t>
+  </si>
+  <si>
+    <t>thêm hóa đơn thành công</t>
+  </si>
+  <si>
+    <t>28.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kiểm tra thêm chi tiết hóa đơn khi chưa nhập số lượng</t>
+  </si>
+  <si>
+    <t>1. Đăng nhập tài khoản Quản lý hoặc Nhân viên bán hàng
+2. Chọn chức năng bán hàng ở màn hình chính
+3. Nhấn hóa đơn
+4. Nhập tên khách hàng hàng
+5. Nhấn Enter trên bàn phím
+6. Chọn ngày
+7. Chọn hàng hóa
+8. Nhập số lượng
+9. Nhấn lưu</t>
+  </si>
+  <si>
+    <t>tên khách hàng: Hoàng Hảo
+ngày: 01/11/2023
+hàng hóa: Coca
+số lượng:</t>
+  </si>
+  <si>
+    <t>28.2</t>
+  </si>
+  <si>
+    <t>Kiểm tra thêm chi tiết hóa đơn khi số lượng không phải số</t>
+  </si>
+  <si>
+    <t>tên khách hàng: Hoàng Hảo
+ngày: 01/11/2023
+hàng hóa: Coca
+số lượng: abc</t>
+  </si>
+  <si>
+    <t>28.3</t>
+  </si>
+  <si>
+    <t>Kiểm tra thêm chi tiết hóa đơn khi số lượng trong kho không đủ</t>
+  </si>
+  <si>
+    <t>tên khách hàng: Hoàng Hảo
+ngày: 01/11/2023
+hàng hóa: Coca
+số lượng: 1000</t>
+  </si>
+  <si>
+    <t>hiện thông báo số lượng không đủ</t>
+  </si>
+  <si>
+    <t>28.4</t>
+  </si>
+  <si>
+    <t>Kiểm tra thêm chi tiết hóa đơn khi số lượng hợp lệ</t>
+  </si>
+  <si>
+    <t>tên khách hàng: Hoàng Hảo
+ngày: 01/11/2023
+hàng hóa: Coca
+số lượng: 2</t>
+  </si>
+  <si>
+    <t>thêm chi tiết hóa đơn thành công và hiển thị chi tiết hóa đơn</t>
+  </si>
+  <si>
+    <t>29.1</t>
+  </si>
+  <si>
+    <t>Kiểm tra áp dụng giảm giá</t>
+  </si>
+  <si>
+    <t>1. Đăng nhập tài khoản Quản lý hoặc Nhân viên bán hàng
+2. Chọn chức năng bán hàng ở màn hình chính
+3. Thêm hóa đơn
+4. Thêm chi tiết hóa đơn
+5. Chọn áp dụng giảm giá hay không
+6. Nhấn xác nhận</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tên khách hàng: Hoàng Hảo
+ngày: 01/11/2023
+hàng hóa: Coca
+số lượng: 2
+áp dụng giảm giá: có
+</t>
+  </si>
+  <si>
+    <t>hiển thị số tiền sau giảm giá</t>
+  </si>
+  <si>
+    <t>30.1</t>
+  </si>
+  <si>
+    <t>Kiểm tra thanh toán khi chưa nhập tiền khách</t>
+  </si>
+  <si>
+    <t>1. Đăng nhập tài khoản Quản lý hoặc Nhân viên bán hàng
+2. Chọn chức năng bán hàng ở màn hình chính
+3. Thêm hóa đơn
+4. Thêm chi tiết hóa đơn
+5. Chọn áp dụng giảm giá hay không
+6. Nhấn xác nhận
+7. Nhập tiền khách
+8. Nhấn thanh toán</t>
+  </si>
+  <si>
+    <t>tên khách hàng: Hoàng Hảo
+ngày: 01/11/2023
+hàng hóa: Coca
+số lượng: 2
+áp dụng giảm giá: có
+tiền của khách:</t>
+  </si>
+  <si>
+    <t>hiện thông báo chưa nhập tiền của khách</t>
+  </si>
+  <si>
+    <t>30.2</t>
+  </si>
+  <si>
+    <t>Kiểm tra thanh toán khi tiền khách không phải số</t>
+  </si>
+  <si>
+    <t>tiền của khách: abc</t>
+  </si>
+  <si>
+    <t>hiện thông báo tiền của khách phải là số</t>
+  </si>
+  <si>
+    <t>30.3</t>
+  </si>
+  <si>
+    <t>Kiểm tra thanh toán khi tiền khách thấp hơn tổng tiền của hóa đơn</t>
+  </si>
+  <si>
+    <t>tên khách hàng: Hoàng Hảo
+ngày: 01/11/2023
+hàng hóa: Coca
+số lượng: 2
+áp dụng giảm giá: có
+tiền của khách: 1</t>
+  </si>
+  <si>
+    <t>hiện thông báo số tiền không hợp lệ</t>
+  </si>
+  <si>
+    <t>30.4</t>
+  </si>
+  <si>
+    <t>Kiểm tra thanh toán khi tiền khách hợp lệ</t>
+  </si>
+  <si>
+    <t>tên khách hàng: Hoàng Hảo
+ngày: 01/11/2023
+hàng hóa: Coca
+số lượng: 2
+áp dụng giảm giá: có
+tiền của khách: 1000000</t>
+  </si>
+  <si>
+    <t>hiện thông báo thanh toán thành công là hiện tiền thối cho khách</t>
+  </si>
+  <si>
+    <t>31.1</t>
+  </si>
+  <si>
+    <t>Kiểm tra xuất hóa đơn</t>
+  </si>
+  <si>
+    <t>1. Đăng nhập tài khoản Quản lý hoặc Nhân viên bán hàng
+2. Chọn chức năng bán hàng ở màn hình chính
+3. Thêm hóa đơn
+4. Thêm chi tiết hóa đơn
+5. Chọn áp dụng giảm giá hay không
+6. Nhấn xác nhận
+7. Nhập tiền khách
+8. Nhấn thanh toán
+9. Nhấn xuất hóa đơn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tên khách hàng: Hoàng Hảo
+ngày: 01/11/2023
+hàng hóa: Coca
+số lượng: 2
+áp dụng giảm giá: có
+tiền khách: 50000
+</t>
+  </si>
+  <si>
+    <t>xuất ra file excel</t>
+  </si>
+  <si>
+    <t>32.1</t>
   </si>
   <si>
     <t>Kiểm tra chức năng hiển thị danh sách phiếu nhập và hóa đơn</t>
@@ -1343,7 +1613,7 @@
     <t>hiển thị danh sách phiếu nhập và danh sách hóa đơn</t>
   </si>
   <si>
-    <t>34.1</t>
+    <t>33.1</t>
   </si>
   <si>
     <t>Kiểm tra thống kê khi chọn ngày thống kê không hợp lệ</t>
@@ -1363,7 +1633,7 @@
     <t>hiện thông báo ngày thống kê không hợp lệ</t>
   </si>
   <si>
-    <t>34.2</t>
+    <t>33.2</t>
   </si>
   <si>
     <t>Kiểm tra thống kê khi dữ liệu hợp lệ</t>
@@ -1394,9 +1664,6 @@
     <t>thống kê từ ngày: 01/01/2023
 thống kê đến ngày: 01/11/2023
 thư mục: Documents</t>
-  </si>
-  <si>
-    <t>xuất ra file excel</t>
   </si>
   <si>
     <r>
@@ -1629,22 +1896,26 @@
 9. Kiểm tra thêm chi tiết phiếu nhập khi để trống ngày sản xuất
 10. Kiểm tra thêm chi tiết phiếu nhập khi để trống hạn sử dụng
 11. Kiểm tra thêm chi tiết phiếu nhập khi ngày sản xuất lớn hơn hạn sử dụng
-12. Kiểm tra thêm chi tiết phiếu nhập khi dữ liệu hợp lệ</t>
+12. Kiểm tra thêm chi tiết phiếu nhập khi hạn sử dụng bé hơn ngày hiện tại
+13. Kiểm tra thêm chi tiết phiếu nhập khi dữ liệu hợp lệ</t>
   </si>
   <si>
     <t>Kiểm tra chức năng thêm hóa đơn</t>
   </si>
   <si>
-    <t>1. Kiểm tra thêm hóa đơn khi khách hàng chưa tồn tại
-2. Kiểm tra thêm hóa đơn khi chưa chọn ngày
-3. Kiểm tra thêm hóa đơn khi dữ liệu hợp lệ</t>
+    <t>1. Kiểm tra thêm hóa đơn khi chưa nhập tên khách hàng
+2. Kiểm tra thêm hóa đơn khi nhập tên khách hàng chưa tồn tại
+3. Kiểm tra thêm hóa đơn khi chưa chọn ngày
+4. Kiểm tra thêm hóa đơn khi dữ liệu hợp lệ</t>
   </si>
   <si>
     <t>Kiểm tra chức năng thêm chi tiết hóa đơn</t>
   </si>
   <si>
-    <t>1. Kiểm tra thêm chi tiết hóa đơn khi số lượng không phải số
-2. Kiểm tra thêm chi tiết hóa đơn khi số lượng hợp lệ</t>
+    <t>1. Kiểm tra thêm chi tiết hóa đơn khi chưa nhập số lượng
+2. Kiểm tra thêm chi tiết hóa đơn khi số lượng không phải số
+3. Kiểm tra thêm chi tiết hóa đơn khi số lượng trong kho không đủ
+4. Kiểm tra thêm chi tiết hóa đơn khi số lượng hợp lệ</t>
   </si>
   <si>
     <t>Kiểm tra chức năng áp dụng giảm giá</t>
@@ -1656,14 +1927,10 @@
     <t>Kiểm tra chức năng thanh toán</t>
   </si>
   <si>
-    <t>1. Kiểm tra thanh toán khi tiền khách không phải số
-2. Kiểm tra thanh toán khi tiền khách thấp hơn tổng tiền của hóa đơn</t>
-  </si>
-  <si>
-    <t>Kiểm tra chức năng hiển thị chi tiết hóa đơn</t>
-  </si>
-  <si>
-    <t>1. Kiểm tra hiển thị chi tiết hóa đơn</t>
+    <t>1. Kiểm tra thanh toán khi chưa nhập tiền khách
+2. Kiểm tra thanh toán khi tiền khách không phải số
+3. Kiểm tra thanh toán khi tiền khách thấp hơn tổng tiền của hóa đơn
+4. Kiểm tra thanh toán khi tiền khách hợp lệ</t>
   </si>
   <si>
     <t>Kiểm tra chức năng xuất hóa đơn</t>
@@ -2890,10 +3157,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:H86"/>
+  <dimension ref="B1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="C90" sqref="C90"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -4720,92 +4987,437 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" ht="72" spans="2:8">
+    <row r="82" ht="216" spans="2:8">
+      <c r="B82" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="83" ht="172.8" spans="2:8">
       <c r="B83" s="3" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>327</v>
+        <v>331</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>332</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="H83" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="84" ht="144" spans="2:8">
+    <row r="84" ht="172.8" spans="2:8">
       <c r="B84" s="3" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>331</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="H84" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="85" ht="144" spans="2:8">
+    <row r="85" ht="172.8" spans="2:8">
       <c r="B85" s="3" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>331</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="H85" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="86" ht="187.2" spans="2:8">
+    <row r="86" ht="172.8" spans="2:8">
       <c r="B86" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="C86" t="s">
-        <v>339</v>
+        <v>342</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>343</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="H86" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87" ht="201.6" spans="2:8">
+      <c r="B87" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="H87" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88" ht="201.6" spans="2:8">
+      <c r="B88" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" ht="201.6" spans="2:8">
+      <c r="B89" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="F89" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90" ht="201.6" spans="2:8">
+      <c r="B90" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="91" ht="144" spans="2:8">
+      <c r="B91" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="H91" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="92" ht="172.8" spans="2:8">
+      <c r="B92" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="93" ht="172.8" spans="2:8">
+      <c r="B93" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="H93" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="94" ht="172.8" spans="2:8">
+      <c r="B94" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95" ht="172.8" spans="2:8">
+      <c r="B95" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="H95" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="96" ht="187.2" spans="2:8">
+      <c r="B96" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="97" ht="72" spans="2:8">
+      <c r="B97" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="H97" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="98" ht="144" spans="2:8">
+      <c r="B98" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="H98" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" ht="144" spans="2:8">
+      <c r="B99" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="H99" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="100" ht="187.2" spans="2:8">
+      <c r="B100" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C100" t="s">
+        <v>402</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="F100" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="H100" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4818,10 +5430,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:D37"/>
+  <dimension ref="B1:D36"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -4837,10 +5449,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>343</v>
+        <v>405</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>344</v>
+        <v>406</v>
       </c>
     </row>
     <row r="3" ht="72" spans="2:4">
@@ -4848,10 +5460,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>345</v>
+        <v>407</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>346</v>
+        <v>408</v>
       </c>
     </row>
     <row r="4" spans="2:4">
@@ -4859,10 +5471,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>347</v>
+        <v>409</v>
       </c>
       <c r="D4" t="s">
-        <v>348</v>
+        <v>410</v>
       </c>
     </row>
     <row r="5" spans="2:4">
@@ -4870,10 +5482,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>349</v>
+        <v>411</v>
       </c>
       <c r="D5" t="s">
-        <v>350</v>
+        <v>412</v>
       </c>
     </row>
     <row r="6" ht="216" spans="2:4">
@@ -4881,10 +5493,10 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>351</v>
+        <v>413</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>352</v>
+        <v>414</v>
       </c>
     </row>
     <row r="7" ht="43.2" spans="2:4">
@@ -4892,10 +5504,10 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>353</v>
+        <v>415</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>354</v>
+        <v>416</v>
       </c>
     </row>
     <row r="8" ht="28.8" spans="2:4">
@@ -4903,10 +5515,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>355</v>
+        <v>417</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>356</v>
+        <v>418</v>
       </c>
     </row>
     <row r="9" spans="2:4">
@@ -4914,10 +5526,10 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>357</v>
+        <v>419</v>
       </c>
       <c r="D9" t="s">
-        <v>358</v>
+        <v>420</v>
       </c>
     </row>
     <row r="10" ht="86.4" spans="2:4">
@@ -4925,10 +5537,10 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>359</v>
+        <v>421</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>360</v>
+        <v>422</v>
       </c>
     </row>
     <row r="11" ht="28.8" spans="2:4">
@@ -4936,10 +5548,10 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>361</v>
+        <v>423</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>362</v>
+        <v>424</v>
       </c>
     </row>
     <row r="12" ht="28.8" spans="2:4">
@@ -4947,10 +5559,10 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>363</v>
+        <v>425</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>364</v>
+        <v>426</v>
       </c>
     </row>
     <row r="13" spans="2:4">
@@ -4958,10 +5570,10 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>365</v>
+        <v>427</v>
       </c>
       <c r="D13" t="s">
-        <v>366</v>
+        <v>428</v>
       </c>
     </row>
     <row r="14" ht="28.8" spans="2:4">
@@ -4969,10 +5581,10 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>367</v>
+        <v>429</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>368</v>
+        <v>430</v>
       </c>
     </row>
     <row r="15" spans="2:4">
@@ -4980,10 +5592,10 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>369</v>
+        <v>431</v>
       </c>
       <c r="D15" t="s">
-        <v>370</v>
+        <v>432</v>
       </c>
     </row>
     <row r="16" spans="2:4">
@@ -4991,10 +5603,10 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>371</v>
+        <v>433</v>
       </c>
       <c r="D16" t="s">
-        <v>372</v>
+        <v>434</v>
       </c>
     </row>
     <row r="17" ht="28.8" spans="2:4">
@@ -5002,10 +5614,10 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>373</v>
+        <v>435</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>374</v>
+        <v>436</v>
       </c>
     </row>
     <row r="18" spans="2:4">
@@ -5013,10 +5625,10 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>375</v>
+        <v>437</v>
       </c>
       <c r="D18" t="s">
-        <v>376</v>
+        <v>438</v>
       </c>
     </row>
     <row r="19" ht="86.4" spans="2:4">
@@ -5024,10 +5636,10 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>377</v>
+        <v>439</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>378</v>
+        <v>440</v>
       </c>
     </row>
     <row r="20" spans="2:4">
@@ -5035,10 +5647,10 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>379</v>
+        <v>441</v>
       </c>
       <c r="D20" t="s">
-        <v>380</v>
+        <v>442</v>
       </c>
     </row>
     <row r="21" ht="28.8" spans="2:4">
@@ -5046,10 +5658,10 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>381</v>
+        <v>443</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>382</v>
+        <v>444</v>
       </c>
     </row>
     <row r="22" spans="2:4">
@@ -5057,10 +5669,10 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>383</v>
+        <v>445</v>
       </c>
       <c r="D22" t="s">
-        <v>384</v>
+        <v>446</v>
       </c>
     </row>
     <row r="23" ht="86.4" spans="2:4">
@@ -5068,10 +5680,10 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>385</v>
+        <v>447</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>386</v>
+        <v>448</v>
       </c>
     </row>
     <row r="24" ht="28.8" spans="2:4">
@@ -5079,10 +5691,10 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>387</v>
+        <v>449</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>388</v>
+        <v>450</v>
       </c>
     </row>
     <row r="25" spans="2:4">
@@ -5090,10 +5702,10 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>389</v>
+        <v>451</v>
       </c>
       <c r="D25" t="s">
-        <v>390</v>
+        <v>452</v>
       </c>
     </row>
     <row r="26" spans="2:4">
@@ -5101,10 +5713,10 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>391</v>
+        <v>453</v>
       </c>
       <c r="D26" t="s">
-        <v>392</v>
+        <v>454</v>
       </c>
     </row>
     <row r="27" spans="2:4">
@@ -5112,43 +5724,43 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>393</v>
+        <v>455</v>
       </c>
       <c r="D27" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="28" ht="172.8" spans="2:4">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="28" ht="187.2" spans="2:4">
       <c r="B28">
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>395</v>
+        <v>457</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="29" ht="43.2" spans="2:4">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="29" ht="57.6" spans="2:4">
       <c r="B29">
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>397</v>
+        <v>459</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="30" ht="28.8" spans="2:4">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="30" ht="57.6" spans="2:4">
       <c r="B30">
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>399</v>
+        <v>461</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>400</v>
+        <v>462</v>
       </c>
     </row>
     <row r="31" spans="2:4">
@@ -5156,21 +5768,21 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>401</v>
+        <v>463</v>
       </c>
       <c r="D31" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="32" ht="28.8" spans="2:4">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="32" ht="57.6" spans="2:4">
       <c r="B32">
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>403</v>
+        <v>465</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>404</v>
+        <v>466</v>
       </c>
     </row>
     <row r="33" spans="2:4">
@@ -5178,10 +5790,10 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>405</v>
+        <v>467</v>
       </c>
       <c r="D33" t="s">
-        <v>406</v>
+        <v>468</v>
       </c>
     </row>
     <row r="34" spans="2:4">
@@ -5189,43 +5801,32 @@
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>407</v>
+        <v>389</v>
       </c>
       <c r="D34" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="35" ht="28.8" spans="2:4">
       <c r="B35">
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>326</v>
-      </c>
-      <c r="D35" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="36" ht="28.8" spans="2:4">
+        <v>470</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4">
       <c r="B36">
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>410</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4">
-      <c r="B37">
-        <v>35</v>
-      </c>
-      <c r="C37" t="s">
-        <v>412</v>
-      </c>
-      <c r="D37" t="s">
-        <v>339</v>
+        <v>472</v>
+      </c>
+      <c r="D36" t="s">
+        <v>402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix lỗi, hoàn thiện thêm testcase
</commit_message>
<xml_diff>
--- a/Kiểm Thử.xlsx
+++ b/Kiểm Thử.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1290" uniqueCount="789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="828">
   <si>
     <r>
       <rPr>
@@ -725,10 +725,28 @@
     <t>5.14</t>
   </si>
   <si>
+    <t>Kiểm tra sửa nhân viên khi sửa chính mình</t>
+  </si>
+  <si>
+    <t>1. Đăng nhập tài khoản Admin hoặc Quản lý
+2. Chọn chức năng nhân viên ở màn hình chính
+3. Chọn chính mình trong danh sách
+4. Nhấn sửa</t>
+  </si>
+  <si>
+    <t>mã nhân viên NV001</t>
+  </si>
+  <si>
+    <t>không cho sửa chức vụ</t>
+  </si>
+  <si>
+    <t>5.15</t>
+  </si>
+  <si>
     <t>Kiểm tra sửa nhân viên khi để trống địa chỉ</t>
   </si>
   <si>
-    <t>5.15</t>
+    <t>5.16</t>
   </si>
   <si>
     <t>Kiểm tra sửa nhân viên khi dữ liệu hợp lệ</t>
@@ -787,6 +805,25 @@
     <t>cho nghỉ nhân viên thành công</t>
   </si>
   <si>
+    <t>6.4</t>
+  </si>
+  <si>
+    <t>Kiểm tra cho nghỉ nhân viên khi cho nghỉ chính mình</t>
+  </si>
+  <si>
+    <t>1. Đăng nhập tài khoản Admin hoặc Quản lý
+2. Chọn chức năng nhân viên ở màn hình chính
+3. Chọn chính mình trong danh sách
+4. Nhấn nghỉ việc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mã nhân viên: NV001
+</t>
+  </si>
+  <si>
+    <t>hiện thông báo không thể cho nghỉ chính mình</t>
+  </si>
+  <si>
     <t>7.1</t>
   </si>
   <si>
@@ -1007,10 +1044,6 @@
 2. Chọn chức năng tài khoản ở màn hình chính
 3. Chọn 1 tài khoản trong danh sách
 4. Nhấn ẩn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mã nhân viên: NV001
-</t>
   </si>
   <si>
     <t>hiện thông báo không thể ẩn tài khoản</t>
@@ -2383,12 +2416,12 @@
     <t>45.1</t>
   </si>
   <si>
-    <t>Kiểm tra tìm kiếm sản phẩm trong kho khi không nhập mã sản phẩm</t>
+    <t>Kiểm tra tìm kiếm sản phẩm trong kho khi không nhập tên sản phẩm</t>
   </si>
   <si>
     <t>1. Đăng nhập tài khoản Quản lý hoặc Nhân viên Kho
 2. Chọn chức năng kho ở màn hình chính
-3. Nhập mã sản phẩm vào ô tìm kiếm
+3. Nhập tên sản phẩm vào ô tìm kiếm
 4. Nhấn tìm kiếm</t>
   </si>
   <si>
@@ -2401,7 +2434,7 @@
     <t>45.2</t>
   </si>
   <si>
-    <t>Kiểm tra tìm kiếm sản phẩm trong kho khi nhập mã sản phẩm không tồn tại</t>
+    <t>Kiểm tra tìm kiếm sản phẩm trong kho khi nhập tên sản phẩm không tồn tại</t>
   </si>
   <si>
     <t>tìm kiếm: abc123</t>
@@ -2413,19 +2446,19 @@
     <t>45.3</t>
   </si>
   <si>
-    <t>Kiểm tra tìm kiếm sản phẩm trong kho khi nhập đúng mã sản phẩm</t>
+    <t>Kiểm tra tìm kiếm sản phẩm trong kho khi nhập đúng tên sản phẩm</t>
   </si>
   <si>
     <t>1. Đăng nhập tài khoản Quản lý hoặc Nhân viên kho
 2. Chọn chức năng kho ở màn hình chính
-3. Nhập mã sản phẩm vào ô tìm kiếm
+3. Nhập tên sản phẩm vào ô tìm kiếm
 4. Nhấn tìm kiếm</t>
   </si>
   <si>
-    <t>tìm kiếm: SP01</t>
-  </si>
-  <si>
-    <t>hiển thị sản phẩm với mã sản phẩm có chứa kí tự muốn tìm kiếm</t>
+    <t>tìm kiếm: cá</t>
+  </si>
+  <si>
+    <t>hiển thị sản phẩm với tên sản phẩm có chứa kí tự muốn tìm kiếm</t>
   </si>
   <si>
     <t>46.1</t>
@@ -2577,12 +2610,12 @@
     <t>50.1</t>
   </si>
   <si>
-    <t>Kiểm tra tìm kiếm tài khoản khi không nhập mã nhân viên</t>
+    <t>Kiểm tra tìm kiếm tài khoản khi không nhập tên nhân viên</t>
   </si>
   <si>
     <t>1. Đăng nhập tài khoản Admin
 2. Chọn chức năng tài khoản ở màn hình chính
-3. Nhập mã nhân viên vào ô tìm kiếm
+3. Nhập tên nhân viên vào ô tìm kiếm
 4. Nhấn tìm kiếm</t>
   </si>
   <si>
@@ -2592,7 +2625,7 @@
     <t>50.2</t>
   </si>
   <si>
-    <t>Kiểm tra tìm kiếm tài khoản khi nhập mã nhân viên không tồn tại</t>
+    <t>Kiểm tra tìm kiếm tài khoản khi nhập tên nhân viên không tồn tại</t>
   </si>
   <si>
     <t>hiện thông báo không tìm thấy tài khoản</t>
@@ -2601,13 +2634,97 @@
     <t>50.3</t>
   </si>
   <si>
-    <t>Kiểm tra tìm kiếm tài khoản khi nhập đúng mã nhân viên</t>
-  </si>
-  <si>
-    <t>tìm kiếm: NV00</t>
-  </si>
-  <si>
-    <t>hiển thị tài khoản với mã nhân viên có chứa kí tự muốn tìm kiếm</t>
+    <t>Kiểm tra tìm kiếm tài khoản khi nhập đúng tên nhân viên</t>
+  </si>
+  <si>
+    <t>tìm kiếm: khôi</t>
+  </si>
+  <si>
+    <t>hiển thị tài khoản với tên nhân viên có chứa kí tự muốn tìm kiếm</t>
+  </si>
+  <si>
+    <t>51.1</t>
+  </si>
+  <si>
+    <t>Kiểm tra hiển thị giao diện khi đăng nhập với quyền admin</t>
+  </si>
+  <si>
+    <t>1. Đăng nhập tài khoản Admin
+2. Chọn các chức năng có trên màn hình</t>
+  </si>
+  <si>
+    <t>tài khoản: ADMIN
+mật khẩu: 123</t>
+  </si>
+  <si>
+    <t>hiển thị giao diện của admin, hiển thị các chức năng admin có thể truy cập</t>
+  </si>
+  <si>
+    <t>51.2</t>
+  </si>
+  <si>
+    <t>Kiểm tra hiển thị giao diện khi đăng nhập với quyền quản lý</t>
+  </si>
+  <si>
+    <t>1. Đăng nhập tài khoản Quản lý
+2. Chọn các chức năng có trên màn hình</t>
+  </si>
+  <si>
+    <t>tài khoản: TRUONGBHX
+mật khẩu: 123</t>
+  </si>
+  <si>
+    <t>hiển thị giao diện của quản lý, hiển thị các chức năng quản lý có thể truy cập</t>
+  </si>
+  <si>
+    <t>51.3</t>
+  </si>
+  <si>
+    <t>Kiểm tra hiển thị giao diện khi đăng nhập với quyền nhân viên bán hàng</t>
+  </si>
+  <si>
+    <t>1. Đăng nhập tài khoản Nhân viên bán hàng
+2. Chọn các chức năng có trên màn hình</t>
+  </si>
+  <si>
+    <t>tài khoản: XINHBHX
+mật khẩu: 123</t>
+  </si>
+  <si>
+    <t>hiển thị giao diện của nhân viên bán hàng, hiển thị các chức năng nhân viên bán hàng có thể truy cập</t>
+  </si>
+  <si>
+    <t>51.4</t>
+  </si>
+  <si>
+    <t>Kiểm tra hiển thị giao diện khi đăng nhập với quyền nhân viên kho</t>
+  </si>
+  <si>
+    <t>1. Đăng nhập tài khoản Nhân viên kho
+2. Chọn các chức năng có trên màn hình</t>
+  </si>
+  <si>
+    <t>tài khoản: NGUYENBHX
+mật khẩu: 123</t>
+  </si>
+  <si>
+    <t>hiển thị giao diện của nhân viên kho, hiển thị các chức năng nhân viên kho có thể truy cập</t>
+  </si>
+  <si>
+    <t>52.1</t>
+  </si>
+  <si>
+    <t>Kiểm tra hủy hóa đơn</t>
+  </si>
+  <si>
+    <t>1. Đăng nhập tài khoản Quản lý hoặc Nhân viên bán hàng
+2. Chọn chức năng hóa đơn trên màn hình chính
+3. Thêm hóa đơn
+4. Thêm chi tiết hóa đơn
+5. Nhấn hủy</t>
+  </si>
+  <si>
+    <t>hủy hóa đơn và không lưu vào cơ sở dữ liệu</t>
   </si>
   <si>
     <r>
@@ -2707,8 +2824,9 @@
 11. Kiểm tra sửa nhân viên khi không chọn ngày vào làm
 12. Kiểm tra sửa nhân viên khi chọn chức vụ Admin với quyền quản lý
 13. Kiểm tra sửa nhân viên khi chọn chức vụ Quản lý với quyền quản lý
-14. Kiểm tra sửa nhân viên khi để trống địa chỉ
-15. Kiểm tra sửa nhân viên khi dữ liệu hợp lệ</t>
+14. Kiểm tra sửa nhân viên khi sửa chính mình
+15. Kiểm tra sửa nhân viên khi để trống địa chỉ
+16. Kiểm tra sửa nhân viên khi dữ liệu hợp lệ</t>
   </si>
   <si>
     <t>TS6</t>
@@ -2718,8 +2836,9 @@
   </si>
   <si>
     <t>1. Kiểm tra cho nghỉ nhân viên có chức vụ Admin với quyền quản lý
-2. Kiểm tra cho nghỉ nhân viên có chức vụ Quản lý với quyền quản lý 
-3. Kiểm tra cho nghỉ nhân viên có chức vụ thấp hơn quyền quản lý</t>
+2. Kiểm tra cho nghỉ nhân viên có chức vụ Quản lý với quyền quản lý
+3. Kiểm tra cho nghỉ nhân viên có chức vụ thấp hơn
+4. Kiểm tra cho nghỉ nhân viên khi cho nghỉ chính mình</t>
   </si>
   <si>
     <t>TS7</t>
@@ -3131,12 +3250,12 @@
     <t>TS45</t>
   </si>
   <si>
-    <t>Kiểm tra chức năng tìm kiếm sản phẩm trong kho theo mã sản phẩm</t>
-  </si>
-  <si>
-    <t>1. Kiểm tra tìm kiếm sản phẩm trong kho khi không nhập mã sản phẩm
-2. Kiểm tra tìm kiếm sản phẩm trong kho khi nhập mã sản phẩm không tồn tại
-3. Kiểm tra tìm kiếm sản phẩm trong kho khi nhập đúng mã sản phẩm</t>
+    <t>Kiểm tra chức năng tìm kiếm sản phẩm trong kho theo tên sản phẩm</t>
+  </si>
+  <si>
+    <t>1. Kiểm tra tìm kiếm sản phẩm trong kho khi không nhập tên sản phẩm
+2. Kiểm tra tìm kiếm sản phẩm trong kho khi nhập tên sản phẩm không tồn tại
+3. Kiểm tra tìm kiếm sản phẩm trong kho khi nhập đúng tên sản phẩm</t>
   </si>
   <si>
     <t>TS46</t>
@@ -3186,12 +3305,33 @@
     <t>TS50</t>
   </si>
   <si>
-    <t>Kiểm tra chức năng tìm kiếm tài khoản theo mã nhân viên</t>
-  </si>
-  <si>
-    <t>1. Kiểm tra tìm kiếm tài khoản khi không nhập mã nhân viên
-2. Kiểm tra tìm kiếm tài khoản khi nhập mã nhân viên không tồn tại
-3. Kiểm tra tìm kiếm tài khoản khi nhập đúng mã nhân viên</t>
+    <t>Kiểm tra chức năng tìm kiếm tài khoản theo tên nhân viên</t>
+  </si>
+  <si>
+    <t>1. Kiểm tra tìm kiếm tài khoản khi không nhập tên nhân viên
+2. Kiểm tra tìm kiếm tài khoản khi nhập tên nhân viên không tồn tại
+3. Kiểm tra tìm kiếm tài khoản khi nhập đúng tên nhân viên</t>
+  </si>
+  <si>
+    <t>TS51</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng hiển thị giao diện khi đăng nhập với các quyền</t>
+  </si>
+  <si>
+    <t>1. Kiểm tra hiển thị giao diện khi đăng nhập với quyền admin
+2. Kiểm tra hiển thị giao diện khi đăng nhập với quyền quản lý
+3. Kiểm tra hiển thị giao diện khi đăng nhập với quyền nhân viên bán hàng
+4. Kiểm tra hiển thị giao diện khi đăng nhập với quyền nhân viên kho</t>
+  </si>
+  <si>
+    <t>TS52</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng hủy hóa đơn</t>
+  </si>
+  <si>
+    <t>1. Kiểm tra hủy hóa đơn</t>
   </si>
 </sst>
 </file>
@@ -3850,7 +3990,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3859,6 +3999,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -4399,10 +4542,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:H165"/>
+  <dimension ref="B1:H172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
-      <selection activeCell="E111" sqref="E111"/>
+    <sheetView tabSelected="1" topLeftCell="A168" workbookViewId="0">
+      <selection activeCell="F176" sqref="F176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -4420,7 +4563,7 @@
   <sheetData>
     <row r="1" ht="15.15"/>
     <row r="2" ht="15.15" spans="2:8">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -5241,7 +5384,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" ht="244.8" spans="2:8">
+    <row r="38" ht="100.8" spans="2:8">
       <c r="B38" s="3" t="s">
         <v>136</v>
       </c>
@@ -5249,16 +5392,16 @@
         <v>137</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>91</v>
+        <v>140</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>91</v>
+        <v>140</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>12</v>
@@ -5266,45 +5409,45 @@
     </row>
     <row r="39" ht="244.8" spans="2:8">
       <c r="B39" s="3" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>98</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>141</v>
+        <v>91</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>141</v>
+        <v>91</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="40" ht="100.8" spans="2:8">
+    <row r="40" ht="244.8" spans="2:8">
       <c r="B40" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>144</v>
+        <v>98</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>145</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>85</v>
+        <v>146</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>85</v>
+        <v>146</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>12</v>
@@ -5312,16 +5455,16 @@
     </row>
     <row r="41" ht="100.8" spans="2:8">
       <c r="B41" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>85</v>
@@ -5335,36 +5478,36 @@
     </row>
     <row r="42" ht="100.8" spans="2:8">
       <c r="B42" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>144</v>
-      </c>
       <c r="E42" s="3" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>152</v>
+        <v>85</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>152</v>
+        <v>85</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="43" ht="86.4" spans="2:8">
+    <row r="43" ht="100.8" spans="2:8">
       <c r="B43" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>156</v>
@@ -5379,7 +5522,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" ht="86.4" spans="2:8">
+    <row r="44" ht="100.8" spans="2:8">
       <c r="B44" s="3" t="s">
         <v>158</v>
       </c>
@@ -5387,79 +5530,82 @@
         <v>159</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="45" ht="57.6" spans="2:8">
+    <row r="45" ht="86.4" spans="2:8">
       <c r="B45" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>166</v>
       </c>
       <c r="F45" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" ht="86.4" spans="2:8">
+      <c r="B46" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="G45" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" ht="115.2" spans="2:8">
-      <c r="B46" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>168</v>
+      <c r="E46" s="3" t="s">
+        <v>170</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="47" ht="115.2" spans="2:8">
+    <row r="47" ht="57.6" spans="2:8">
       <c r="B47" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>11</v>
+        <v>175</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>11</v>
+        <v>175</v>
       </c>
       <c r="H47" s="3" t="s">
         <v>12</v>
@@ -5467,22 +5613,19 @@
     </row>
     <row r="48" ht="115.2" spans="2:8">
       <c r="B48" s="3" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>12</v>
@@ -5490,22 +5633,22 @@
     </row>
     <row r="49" ht="115.2" spans="2:8">
       <c r="B49" s="3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C49" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>168</v>
-      </c>
       <c r="E49" s="3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>180</v>
+        <v>11</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>180</v>
+        <v>11</v>
       </c>
       <c r="H49" s="3" t="s">
         <v>12</v>
@@ -5513,22 +5656,22 @@
     </row>
     <row r="50" ht="115.2" spans="2:8">
       <c r="B50" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>16</v>
+        <v>186</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>16</v>
+        <v>186</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>12</v>
@@ -5536,22 +5679,22 @@
     </row>
     <row r="51" ht="115.2" spans="2:8">
       <c r="B51" s="3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>12</v>
@@ -5559,68 +5702,68 @@
     </row>
     <row r="52" ht="115.2" spans="2:8">
       <c r="B52" s="3" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>191</v>
+        <v>16</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>191</v>
+        <v>16</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="53" ht="144" spans="2:8">
+    <row r="53" ht="115.2" spans="2:8">
       <c r="B53" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>11</v>
+        <v>197</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>11</v>
+        <v>197</v>
       </c>
       <c r="H53" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="54" ht="144" spans="2:8">
+    <row r="54" ht="115.2" spans="2:8">
       <c r="B54" s="3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>12</v>
@@ -5628,22 +5771,22 @@
     </row>
     <row r="55" ht="144" spans="2:8">
       <c r="B55" s="3" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>180</v>
+        <v>11</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>180</v>
+        <v>11</v>
       </c>
       <c r="H55" s="3" t="s">
         <v>12</v>
@@ -5651,22 +5794,22 @@
     </row>
     <row r="56" ht="144" spans="2:8">
       <c r="B56" s="3" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>16</v>
+        <v>186</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>16</v>
+        <v>186</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>12</v>
@@ -5674,22 +5817,22 @@
     </row>
     <row r="57" ht="144" spans="2:8">
       <c r="B57" s="3" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="H57" s="3" t="s">
         <v>12</v>
@@ -5697,85 +5840,85 @@
     </row>
     <row r="58" ht="144" spans="2:8">
       <c r="B58" s="3" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>211</v>
+        <v>16</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>211</v>
+        <v>16</v>
       </c>
       <c r="H58" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="59" ht="100.8" spans="2:8">
+    <row r="59" ht="144" spans="2:8">
       <c r="B59" s="3" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
       <c r="H59" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="60" ht="100.8" spans="2:8">
+    <row r="60" ht="144" spans="2:8">
       <c r="B60" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="61" ht="86.4" spans="2:8">
+    <row r="61" ht="100.8" spans="2:8">
       <c r="B61" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>224</v>
+        <v>161</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>225</v>
@@ -5787,7 +5930,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" ht="86.4" spans="2:8">
+    <row r="62" ht="100.8" spans="2:8">
       <c r="B62" s="3" t="s">
         <v>226</v>
       </c>
@@ -5795,7 +5938,7 @@
         <v>227</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>228</v>
@@ -5820,25 +5963,28 @@
       <c r="D63" s="3" t="s">
         <v>232</v>
       </c>
+      <c r="E63" s="3" t="s">
+        <v>233</v>
+      </c>
       <c r="F63" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="H63" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="64" ht="144" spans="2:8">
+    <row r="64" ht="86.4" spans="2:8">
       <c r="B64" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>237</v>
@@ -5853,7 +5999,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" ht="144" spans="2:8">
+    <row r="65" ht="86.4" spans="2:8">
       <c r="B65" s="3" t="s">
         <v>239</v>
       </c>
@@ -5861,9 +6007,6 @@
         <v>240</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="E65" s="3" t="s">
         <v>241</v>
       </c>
       <c r="F65" s="3" t="s">
@@ -5884,30 +6027,30 @@
         <v>244</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="E66" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" ht="144" spans="2:8">
+      <c r="B67" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D67" s="3" t="s">
         <v>245</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="H66" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="67" ht="129.6" spans="2:8">
-      <c r="B67" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>249</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>250</v>
@@ -5922,7 +6065,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" ht="115.2" spans="2:8">
+    <row r="68" ht="144" spans="2:8">
       <c r="B68" s="3" t="s">
         <v>252</v>
       </c>
@@ -5930,30 +6073,30 @@
         <v>253</v>
       </c>
       <c r="D68" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E68" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="F68" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="F68" s="3" t="s">
+      <c r="G68" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" ht="129.6" spans="2:8">
+      <c r="B69" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="G68" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="H68" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="69" ht="115.2" spans="2:8">
-      <c r="B69" s="3" t="s">
+      <c r="C69" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="D69" s="3" t="s">
         <v>258</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>254</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>259</v>
@@ -5968,7 +6111,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" ht="129.6" spans="2:8">
+    <row r="70" ht="115.2" spans="2:8">
       <c r="B70" s="3" t="s">
         <v>261</v>
       </c>
@@ -5991,7 +6134,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" ht="129.6" spans="2:8">
+    <row r="71" ht="115.2" spans="2:8">
       <c r="B71" s="3" t="s">
         <v>266</v>
       </c>
@@ -5999,6 +6142,9 @@
         <v>267</v>
       </c>
       <c r="D71" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E71" s="3" t="s">
         <v>268</v>
       </c>
       <c r="F71" s="3" t="s">
@@ -6011,7 +6157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" ht="158.4" spans="2:8">
+    <row r="72" ht="129.6" spans="2:8">
       <c r="B72" s="3" t="s">
         <v>270</v>
       </c>
@@ -6034,7 +6180,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="73" ht="158.4" spans="2:8">
+    <row r="73" ht="129.6" spans="2:8">
       <c r="B73" s="3" t="s">
         <v>275</v>
       </c>
@@ -6042,9 +6188,6 @@
         <v>276</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="E73" s="3" t="s">
         <v>277</v>
       </c>
       <c r="F73" s="3" t="s">
@@ -6065,62 +6208,62 @@
         <v>280</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="E74" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="H74" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" ht="158.4" spans="2:8">
+      <c r="B75" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D75" s="3" t="s">
         <v>281</v>
-      </c>
-      <c r="F74" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="H74" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="75" ht="187.2" spans="2:8">
-      <c r="B75" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>285</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>286</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="H75" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="76" ht="187.2" spans="2:8">
+    <row r="76" ht="158.4" spans="2:8">
       <c r="B76" s="3" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="H76" s="3" t="s">
         <v>12</v>
@@ -6128,51 +6271,51 @@
     </row>
     <row r="77" ht="187.2" spans="2:8">
       <c r="B77" s="3" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="H77" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="78" ht="158.4" spans="2:8">
+    <row r="78" ht="187.2" spans="2:8">
       <c r="B78" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="D78" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="C78" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>296</v>
-      </c>
       <c r="E78" s="3" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="H78" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="79" ht="100.8" spans="2:8">
+    <row r="79" ht="187.2" spans="2:8">
       <c r="B79" s="3" t="s">
         <v>299</v>
       </c>
@@ -6180,6 +6323,9 @@
         <v>300</v>
       </c>
       <c r="D79" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="E79" s="3" t="s">
         <v>301</v>
       </c>
       <c r="F79" s="3" t="s">
@@ -6192,7 +6338,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" ht="187.2" spans="2:8">
+    <row r="80" ht="158.4" spans="2:8">
       <c r="B80" s="3" t="s">
         <v>303</v>
       </c>
@@ -6215,7 +6361,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" ht="187.2" spans="2:8">
+    <row r="81" ht="100.8" spans="2:8">
       <c r="B81" s="3" t="s">
         <v>308</v>
       </c>
@@ -6223,9 +6369,6 @@
         <v>309</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="E81" s="3" t="s">
         <v>310</v>
       </c>
       <c r="F81" s="3" t="s">
@@ -6246,16 +6389,16 @@
         <v>313</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>91</v>
+        <v>316</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>91</v>
+        <v>316</v>
       </c>
       <c r="H82" s="3" t="s">
         <v>12</v>
@@ -6263,22 +6406,22 @@
     </row>
     <row r="83" ht="187.2" spans="2:8">
       <c r="B83" s="3" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>69</v>
+        <v>320</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>69</v>
+        <v>320</v>
       </c>
       <c r="H83" s="3" t="s">
         <v>12</v>
@@ -6286,22 +6429,22 @@
     </row>
     <row r="84" ht="187.2" spans="2:8">
       <c r="B84" s="3" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="H84" s="3" t="s">
         <v>12</v>
@@ -6309,22 +6452,22 @@
     </row>
     <row r="85" ht="187.2" spans="2:8">
       <c r="B85" s="3" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H85" s="3" t="s">
         <v>12</v>
@@ -6332,68 +6475,68 @@
     </row>
     <row r="86" ht="187.2" spans="2:8">
       <c r="B86" s="3" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>327</v>
+        <v>73</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>327</v>
+        <v>73</v>
       </c>
       <c r="H86" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="87" ht="216" spans="2:8">
+    <row r="87" ht="187.2" spans="2:8">
       <c r="B87" s="3" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>307</v>
+        <v>77</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>307</v>
+        <v>77</v>
       </c>
       <c r="H87" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="88" ht="216" spans="2:8">
+    <row r="88" ht="187.2" spans="2:8">
       <c r="B88" s="3" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>311</v>
+        <v>336</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>311</v>
+        <v>336</v>
       </c>
       <c r="H88" s="3" t="s">
         <v>12</v>
@@ -6401,22 +6544,22 @@
     </row>
     <row r="89" ht="216" spans="2:8">
       <c r="B89" s="3" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>91</v>
+        <v>316</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>91</v>
+        <v>316</v>
       </c>
       <c r="H89" s="3" t="s">
         <v>12</v>
@@ -6424,22 +6567,22 @@
     </row>
     <row r="90" ht="216" spans="2:8">
       <c r="B90" s="3" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="C90" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="D90" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="D90" s="3" t="s">
-        <v>330</v>
-      </c>
       <c r="E90" s="3" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>69</v>
+        <v>320</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>69</v>
+        <v>320</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>12</v>
@@ -6447,22 +6590,22 @@
     </row>
     <row r="91" ht="216" spans="2:8">
       <c r="B91" s="3" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="H91" s="3" t="s">
         <v>12</v>
@@ -6470,22 +6613,22 @@
     </row>
     <row r="92" ht="216" spans="2:8">
       <c r="B92" s="3" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H92" s="3" t="s">
         <v>12</v>
@@ -6493,51 +6636,51 @@
     </row>
     <row r="93" ht="216" spans="2:8">
       <c r="B93" s="3" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>350</v>
+        <v>73</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>350</v>
+        <v>73</v>
       </c>
       <c r="H93" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="94" ht="144" spans="2:8">
+    <row r="94" ht="216" spans="2:8">
       <c r="B94" s="3" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>353</v>
+        <v>339</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>355</v>
+        <v>77</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>355</v>
+        <v>77</v>
       </c>
       <c r="H94" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="95" ht="72" spans="2:8">
+    <row r="95" ht="216" spans="2:8">
       <c r="B95" s="3" t="s">
         <v>356</v>
       </c>
@@ -6545,6 +6688,9 @@
         <v>357</v>
       </c>
       <c r="D95" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="E95" s="3" t="s">
         <v>358</v>
       </c>
       <c r="F95" s="3" t="s">
@@ -6557,7 +6703,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" ht="100.8" spans="2:8">
+    <row r="96" ht="144" spans="2:8">
       <c r="B96" s="3" t="s">
         <v>360</v>
       </c>
@@ -6580,7 +6726,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" ht="100.8" spans="2:8">
+    <row r="97" ht="72" spans="2:8">
       <c r="B97" s="3" t="s">
         <v>365</v>
       </c>
@@ -6588,9 +6734,6 @@
         <v>366</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="E97" s="3" t="s">
         <v>367</v>
       </c>
       <c r="F97" s="3" t="s">
@@ -6603,7 +6746,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" ht="86.4" spans="2:8">
+    <row r="98" ht="100.8" spans="2:8">
       <c r="B98" s="3" t="s">
         <v>369</v>
       </c>
@@ -6613,57 +6756,57 @@
       <c r="D98" s="3" t="s">
         <v>371</v>
       </c>
+      <c r="E98" s="3" t="s">
+        <v>372</v>
+      </c>
       <c r="F98" s="3" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="H98" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="99" ht="144" spans="2:8">
+    <row r="99" ht="100.8" spans="2:8">
       <c r="B99" s="3" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>376</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>41</v>
+        <v>377</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>41</v>
+        <v>377</v>
       </c>
       <c r="H99" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="100" ht="144" spans="2:8">
+    <row r="100" ht="86.4" spans="2:8">
       <c r="B100" s="3" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>45</v>
+        <v>381</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>45</v>
+        <v>381</v>
       </c>
       <c r="H100" s="3" t="s">
         <v>12</v>
@@ -6671,22 +6814,22 @@
     </row>
     <row r="101" ht="144" spans="2:8">
       <c r="B101" s="3" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="H101" s="3" t="s">
         <v>12</v>
@@ -6694,22 +6837,22 @@
     </row>
     <row r="102" ht="144" spans="2:8">
       <c r="B102" s="3" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="C102" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="D102" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="D102" s="3" t="s">
-        <v>375</v>
-      </c>
       <c r="E102" s="3" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="H102" s="3" t="s">
         <v>12</v>
@@ -6717,22 +6860,22 @@
     </row>
     <row r="103" ht="144" spans="2:8">
       <c r="B103" s="3" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H103" s="3" t="s">
         <v>12</v>
@@ -6740,68 +6883,68 @@
     </row>
     <row r="104" ht="144" spans="2:8">
       <c r="B104" s="3" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>392</v>
+        <v>73</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>392</v>
+        <v>73</v>
       </c>
       <c r="H104" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="105" ht="172.8" spans="2:8">
+    <row r="105" ht="144" spans="2:8">
       <c r="B105" s="3" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="H105" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="106" ht="172.8" spans="2:8">
+    <row r="106" ht="144" spans="2:8">
       <c r="B106" s="3" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>45</v>
+        <v>401</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>45</v>
+        <v>401</v>
       </c>
       <c r="H106" s="3" t="s">
         <v>12</v>
@@ -6809,22 +6952,22 @@
     </row>
     <row r="107" ht="172.8" spans="2:8">
       <c r="B107" s="3" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="H107" s="3" t="s">
         <v>12</v>
@@ -6832,22 +6975,22 @@
     </row>
     <row r="108" ht="172.8" spans="2:8">
       <c r="B108" s="3" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="C108" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="D108" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="D108" s="3" t="s">
-        <v>395</v>
-      </c>
       <c r="E108" s="3" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="H108" s="3" t="s">
         <v>12</v>
@@ -6855,22 +6998,22 @@
     </row>
     <row r="109" ht="172.8" spans="2:8">
       <c r="B109" s="3" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H109" s="3" t="s">
         <v>12</v>
@@ -6878,51 +7021,51 @@
     </row>
     <row r="110" ht="172.8" spans="2:8">
       <c r="B110" s="3" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>412</v>
+        <v>73</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>412</v>
+        <v>73</v>
       </c>
       <c r="H110" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="111" ht="129.6" spans="2:8">
+    <row r="111" ht="172.8" spans="2:8">
       <c r="B111" s="3" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>415</v>
+        <v>404</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>417</v>
+        <v>77</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>417</v>
+        <v>77</v>
       </c>
       <c r="H111" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="112" ht="115.2" spans="2:8">
+    <row r="112" ht="172.8" spans="2:8">
       <c r="B112" s="3" t="s">
         <v>418</v>
       </c>
@@ -6930,30 +7073,30 @@
         <v>419</v>
       </c>
       <c r="D112" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="E112" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="E112" s="3" t="s">
+      <c r="F112" s="3" t="s">
         <v>421</v>
       </c>
-      <c r="F112" s="3" t="s">
+      <c r="G112" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="H112" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="113" ht="129.6" spans="2:8">
+      <c r="B113" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="G112" s="3" t="s">
-        <v>422</v>
-      </c>
-      <c r="H112" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="113" ht="115.2" spans="2:8">
-      <c r="B113" s="3" t="s">
+      <c r="C113" s="3" t="s">
         <v>423</v>
       </c>
-      <c r="C113" s="3" t="s">
+      <c r="D113" s="3" t="s">
         <v>424</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>420</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>425</v>
@@ -6968,7 +7111,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="114" ht="72" spans="2:8">
+    <row r="114" ht="115.2" spans="2:8">
       <c r="B114" s="3" t="s">
         <v>427</v>
       </c>
@@ -6978,11 +7121,14 @@
       <c r="D114" s="3" t="s">
         <v>429</v>
       </c>
+      <c r="E114" s="3" t="s">
+        <v>430</v>
+      </c>
       <c r="F114" s="3" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="H114" s="3" t="s">
         <v>12</v>
@@ -6990,13 +7136,13 @@
     </row>
     <row r="115" ht="115.2" spans="2:8">
       <c r="B115" s="3" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>434</v>
@@ -7011,7 +7157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="116" ht="100.8" spans="2:8">
+    <row r="116" ht="72" spans="2:8">
       <c r="B116" s="3" t="s">
         <v>436</v>
       </c>
@@ -7021,14 +7167,11 @@
       <c r="D116" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="E116" s="3" t="s">
+      <c r="F116" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="F116" s="3" t="s">
-        <v>440</v>
-      </c>
       <c r="G116" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H116" s="3" t="s">
         <v>12</v>
@@ -7036,16 +7179,16 @@
     </row>
     <row r="117" ht="115.2" spans="2:8">
       <c r="B117" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="C117" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="C117" s="3" t="s">
+      <c r="D117" s="3" t="s">
         <v>442</v>
       </c>
-      <c r="D117" s="3" t="s">
+      <c r="E117" s="3" t="s">
         <v>443</v>
-      </c>
-      <c r="E117" s="3" t="s">
-        <v>439</v>
       </c>
       <c r="F117" s="3" t="s">
         <v>444</v>
@@ -7057,7 +7200,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="118" ht="216" spans="2:8">
+    <row r="118" ht="100.8" spans="2:8">
       <c r="B118" s="3" t="s">
         <v>445</v>
       </c>
@@ -7080,7 +7223,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="119" ht="216" spans="2:8">
+    <row r="119" ht="115.2" spans="2:8">
       <c r="B119" s="3" t="s">
         <v>450</v>
       </c>
@@ -7088,16 +7231,16 @@
         <v>451</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>447</v>
+        <v>452</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>242</v>
+        <v>453</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>242</v>
+        <v>453</v>
       </c>
       <c r="H119" s="3" t="s">
         <v>12</v>
@@ -7105,22 +7248,22 @@
     </row>
     <row r="120" ht="216" spans="2:8">
       <c r="B120" s="3" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>447</v>
+        <v>456</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="H120" s="3" t="s">
         <v>12</v>
@@ -7128,22 +7271,22 @@
     </row>
     <row r="121" ht="216" spans="2:8">
       <c r="B121" s="3" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>447</v>
+        <v>456</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>460</v>
+        <v>251</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>460</v>
+        <v>251</v>
       </c>
       <c r="H121" s="3" t="s">
         <v>12</v>
@@ -7151,22 +7294,22 @@
     </row>
     <row r="122" ht="216" spans="2:8">
       <c r="B122" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>447</v>
+        <v>456</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="H122" s="3" t="s">
         <v>12</v>
@@ -7174,22 +7317,22 @@
     </row>
     <row r="123" ht="216" spans="2:8">
       <c r="B123" s="3" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>447</v>
+        <v>456</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="G123" s="3" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="H123" s="3" t="s">
         <v>12</v>
@@ -7197,22 +7340,22 @@
     </row>
     <row r="124" ht="216" spans="2:8">
       <c r="B124" s="3" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>447</v>
+        <v>456</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="H124" s="3" t="s">
         <v>12</v>
@@ -7220,22 +7363,22 @@
     </row>
     <row r="125" ht="216" spans="2:8">
       <c r="B125" s="3" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>447</v>
+        <v>456</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="H125" s="3" t="s">
         <v>12</v>
@@ -7243,22 +7386,22 @@
     </row>
     <row r="126" ht="216" spans="2:8">
       <c r="B126" s="3" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>447</v>
+        <v>456</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="H126" s="3" t="s">
         <v>12</v>
@@ -7266,22 +7409,22 @@
     </row>
     <row r="127" ht="216" spans="2:8">
       <c r="B127" s="3" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>447</v>
+        <v>456</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="H127" s="3" t="s">
         <v>12</v>
@@ -7289,22 +7432,22 @@
     </row>
     <row r="128" ht="216" spans="2:8">
       <c r="B128" s="3" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>447</v>
+        <v>456</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="H128" s="3" t="s">
         <v>12</v>
@@ -7312,36 +7455,36 @@
     </row>
     <row r="129" ht="216" spans="2:8">
       <c r="B129" s="3" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>447</v>
+        <v>456</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="H129" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="130" ht="172.8" spans="2:8">
+    <row r="130" ht="216" spans="2:8">
       <c r="B130" s="3" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>495</v>
+        <v>456</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>496</v>
@@ -7356,7 +7499,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="131" ht="172.8" spans="2:8">
+    <row r="131" ht="216" spans="2:8">
       <c r="B131" s="3" t="s">
         <v>498</v>
       </c>
@@ -7364,7 +7507,7 @@
         <v>499</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>495</v>
+        <v>456</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>500</v>
@@ -7387,16 +7530,16 @@
         <v>503</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>495</v>
+        <v>504</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="H132" s="3" t="s">
         <v>12</v>
@@ -7404,68 +7547,68 @@
     </row>
     <row r="133" ht="172.8" spans="2:8">
       <c r="B133" s="3" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>495</v>
+        <v>504</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="G133" s="3" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="H133" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="134" ht="201.6" spans="2:8">
+    <row r="134" ht="172.8" spans="2:8">
       <c r="B134" s="3" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>513</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>456</v>
+        <v>514</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>456</v>
+        <v>514</v>
       </c>
       <c r="H134" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="135" ht="201.6" spans="2:8">
+    <row r="135" ht="172.8" spans="2:8">
       <c r="B135" s="3" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>460</v>
+        <v>518</v>
       </c>
       <c r="G135" s="3" t="s">
-        <v>460</v>
+        <v>518</v>
       </c>
       <c r="H135" s="3" t="s">
         <v>12</v>
@@ -7473,22 +7616,22 @@
     </row>
     <row r="136" ht="201.6" spans="2:8">
       <c r="B136" s="3" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>512</v>
+        <v>521</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>520</v>
+        <v>465</v>
       </c>
       <c r="G136" s="3" t="s">
-        <v>520</v>
+        <v>465</v>
       </c>
       <c r="H136" s="3" t="s">
         <v>12</v>
@@ -7496,36 +7639,36 @@
     </row>
     <row r="137" ht="201.6" spans="2:8">
       <c r="B137" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="D137" s="3" t="s">
         <v>521</v>
       </c>
-      <c r="C137" s="3" t="s">
-        <v>522</v>
-      </c>
-      <c r="D137" s="3" t="s">
-        <v>512</v>
-      </c>
       <c r="E137" s="3" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>524</v>
+        <v>469</v>
       </c>
       <c r="G137" s="3" t="s">
-        <v>524</v>
+        <v>469</v>
       </c>
       <c r="H137" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="138" ht="144" spans="2:8">
+    <row r="138" ht="201.6" spans="2:8">
       <c r="B138" s="3" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>528</v>
@@ -7540,7 +7683,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="139" ht="172.8" spans="2:8">
+    <row r="139" ht="201.6" spans="2:8">
       <c r="B139" s="3" t="s">
         <v>530</v>
       </c>
@@ -7548,30 +7691,30 @@
         <v>531</v>
       </c>
       <c r="D139" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="E139" s="3" t="s">
         <v>532</v>
       </c>
-      <c r="E139" s="3" t="s">
+      <c r="F139" s="3" t="s">
         <v>533</v>
       </c>
-      <c r="F139" s="3" t="s">
+      <c r="G139" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="H139" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="140" ht="144" spans="2:8">
+      <c r="B140" s="3" t="s">
         <v>534</v>
       </c>
-      <c r="G139" s="3" t="s">
-        <v>534</v>
-      </c>
-      <c r="H139" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="140" ht="172.8" spans="2:8">
-      <c r="B140" s="3" t="s">
+      <c r="C140" s="3" t="s">
         <v>535</v>
       </c>
-      <c r="C140" s="3" t="s">
+      <c r="D140" s="3" t="s">
         <v>536</v>
-      </c>
-      <c r="D140" s="3" t="s">
-        <v>532</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>537</v>
@@ -7594,16 +7737,16 @@
         <v>540</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>532</v>
+        <v>541</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="G141" s="3" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="H141" s="3" t="s">
         <v>12</v>
@@ -7611,36 +7754,36 @@
     </row>
     <row r="142" ht="172.8" spans="2:8">
       <c r="B142" s="3" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>532</v>
+        <v>541</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="G142" s="3" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="H142" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="143" ht="187.2" spans="2:8">
+    <row r="143" ht="172.8" spans="2:8">
       <c r="B143" s="3" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>550</v>
@@ -7655,7 +7798,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="144" ht="72" spans="2:8">
+    <row r="144" ht="172.8" spans="2:8">
       <c r="B144" s="3" t="s">
         <v>552</v>
       </c>
@@ -7663,6 +7806,9 @@
         <v>553</v>
       </c>
       <c r="D144" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="E144" s="3" t="s">
         <v>554</v>
       </c>
       <c r="F144" s="3" t="s">
@@ -7675,7 +7821,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="145" ht="144" spans="2:8">
+    <row r="145" ht="187.2" spans="2:8">
       <c r="B145" s="3" t="s">
         <v>556</v>
       </c>
@@ -7698,7 +7844,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="146" ht="144" spans="2:8">
+    <row r="146" ht="72" spans="2:8">
       <c r="B146" s="3" t="s">
         <v>561</v>
       </c>
@@ -7706,9 +7852,6 @@
         <v>562</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>558</v>
-      </c>
-      <c r="E146" s="3" t="s">
         <v>563</v>
       </c>
       <c r="F146" s="3" t="s">
@@ -7721,7 +7864,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="147" ht="187.2" spans="2:8">
+    <row r="147" ht="144" spans="2:8">
       <c r="B147" s="3" t="s">
         <v>565</v>
       </c>
@@ -7735,24 +7878,24 @@
         <v>568</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>551</v>
+        <v>569</v>
       </c>
       <c r="G147" s="3" t="s">
-        <v>551</v>
+        <v>569</v>
       </c>
       <c r="H147" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="148" ht="115.2" spans="2:8">
+    <row r="148" ht="144" spans="2:8">
       <c r="B148" s="3" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>572</v>
@@ -7767,7 +7910,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" ht="115.2" spans="2:8">
+    <row r="149" ht="187.2" spans="2:8">
       <c r="B149" s="3" t="s">
         <v>574</v>
       </c>
@@ -7775,16 +7918,16 @@
         <v>575</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>571</v>
+        <v>576</v>
       </c>
       <c r="E149" s="3" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="F149" s="3" t="s">
-        <v>577</v>
+        <v>560</v>
       </c>
       <c r="G149" s="3" t="s">
-        <v>577</v>
+        <v>560</v>
       </c>
       <c r="H149" s="3" t="s">
         <v>12</v>
@@ -7813,7 +7956,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="151" ht="158.4" spans="2:8">
+    <row r="151" ht="115.2" spans="2:8">
       <c r="B151" s="3" t="s">
         <v>583</v>
       </c>
@@ -7821,10 +7964,10 @@
         <v>584</v>
       </c>
       <c r="D151" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="E151" s="3" t="s">
         <v>585</v>
-      </c>
-      <c r="E151" s="3" t="s">
-        <v>572</v>
       </c>
       <c r="F151" s="3" t="s">
         <v>586</v>
@@ -7836,7 +7979,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="152" ht="158.4" spans="2:8">
+    <row r="152" ht="115.2" spans="2:8">
       <c r="B152" s="3" t="s">
         <v>587</v>
       </c>
@@ -7844,16 +7987,16 @@
         <v>588</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>585</v>
+        <v>589</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>576</v>
+        <v>590</v>
       </c>
       <c r="F152" s="3" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="G152" s="3" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="H152" s="3" t="s">
         <v>12</v>
@@ -7861,68 +8004,68 @@
     </row>
     <row r="153" ht="158.4" spans="2:8">
       <c r="B153" s="3" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="D153" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="E153" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="F153" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="G153" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="H153" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="154" ht="158.4" spans="2:8">
+      <c r="B154" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>597</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="E154" s="3" t="s">
         <v>585</v>
       </c>
-      <c r="E153" s="3" t="s">
-        <v>592</v>
-      </c>
-      <c r="F153" s="3" t="s">
-        <v>593</v>
-      </c>
-      <c r="G153" s="3" t="s">
-        <v>593</v>
-      </c>
-      <c r="H153" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="154" ht="144" spans="2:8">
-      <c r="B154" s="3" t="s">
+      <c r="F154" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="G154" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="H154" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="155" ht="158.4" spans="2:8">
+      <c r="B155" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D155" s="3" t="s">
         <v>594</v>
       </c>
-      <c r="C154" s="3" t="s">
-        <v>595</v>
-      </c>
-      <c r="D154" s="3" t="s">
-        <v>596</v>
-      </c>
-      <c r="E154" s="3" t="s">
-        <v>572</v>
-      </c>
-      <c r="F154" s="3" t="s">
-        <v>597</v>
-      </c>
-      <c r="G154" s="3" t="s">
-        <v>597</v>
-      </c>
-      <c r="H154" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="155" ht="144" spans="2:8">
-      <c r="B155" s="3" t="s">
-        <v>598</v>
-      </c>
-      <c r="C155" s="3" t="s">
-        <v>599</v>
-      </c>
-      <c r="D155" s="3" t="s">
-        <v>596</v>
-      </c>
       <c r="E155" s="3" t="s">
-        <v>576</v>
+        <v>601</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="G155" s="3" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="H155" s="3" t="s">
         <v>12</v>
@@ -7930,68 +8073,68 @@
     </row>
     <row r="156" ht="144" spans="2:8">
       <c r="B156" s="3" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>596</v>
+        <v>605</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>603</v>
+        <v>581</v>
       </c>
       <c r="F156" s="3" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="G156" s="3" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="H156" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="157" ht="115.2" spans="2:8">
+    <row r="157" ht="144" spans="2:8">
       <c r="B157" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="D157" s="3" t="s">
         <v>605</v>
       </c>
-      <c r="C157" s="3" t="s">
-        <v>606</v>
-      </c>
-      <c r="D157" s="3" t="s">
-        <v>607</v>
-      </c>
       <c r="E157" s="3" t="s">
-        <v>572</v>
+        <v>585</v>
       </c>
       <c r="F157" s="3" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="G157" s="3" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="H157" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="158" ht="115.2" spans="2:8">
+    <row r="158" ht="144" spans="2:8">
       <c r="B158" s="3" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="E158" s="3" t="s">
-        <v>576</v>
+        <v>612</v>
       </c>
       <c r="F158" s="3" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="G158" s="3" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="H158" s="3" t="s">
         <v>12</v>
@@ -7999,68 +8142,68 @@
     </row>
     <row r="159" ht="115.2" spans="2:8">
       <c r="B159" s="3" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>607</v>
+        <v>616</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>614</v>
+        <v>581</v>
       </c>
       <c r="F159" s="3" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="G159" s="3" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="H159" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="160" ht="100.8" spans="2:8">
+    <row r="160" ht="115.2" spans="2:8">
       <c r="B160" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="D160" s="3" t="s">
         <v>616</v>
       </c>
-      <c r="C160" s="3" t="s">
-        <v>617</v>
-      </c>
-      <c r="D160" s="3" t="s">
-        <v>618</v>
-      </c>
       <c r="E160" s="3" t="s">
-        <v>572</v>
+        <v>585</v>
       </c>
       <c r="F160" s="3" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="G160" s="3" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="H160" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="161" ht="100.8" spans="2:8">
+    <row r="161" ht="115.2" spans="2:8">
       <c r="B161" s="3" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>576</v>
+        <v>623</v>
       </c>
       <c r="F161" s="3" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="G161" s="3" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="H161" s="3" t="s">
         <v>12</v>
@@ -8068,22 +8211,22 @@
     </row>
     <row r="162" ht="100.8" spans="2:8">
       <c r="B162" s="3" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>618</v>
+        <v>627</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>625</v>
+        <v>581</v>
       </c>
       <c r="F162" s="3" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="G162" s="3" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="H162" s="3" t="s">
         <v>12</v>
@@ -8091,22 +8234,22 @@
     </row>
     <row r="163" ht="100.8" spans="2:8">
       <c r="B163" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>630</v>
+      </c>
+      <c r="D163" s="3" t="s">
         <v>627</v>
       </c>
-      <c r="C163" s="3" t="s">
-        <v>628</v>
-      </c>
-      <c r="D163" s="3" t="s">
-        <v>629</v>
-      </c>
       <c r="E163" s="3" t="s">
-        <v>572</v>
+        <v>585</v>
       </c>
       <c r="F163" s="3" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="G163" s="3" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="H163" s="3" t="s">
         <v>12</v>
@@ -8114,22 +8257,22 @@
     </row>
     <row r="164" ht="100.8" spans="2:8">
       <c r="B164" s="3" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>576</v>
+        <v>634</v>
       </c>
       <c r="F164" s="3" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="G164" s="3" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="H164" s="3" t="s">
         <v>12</v>
@@ -8137,24 +8280,182 @@
     </row>
     <row r="165" ht="100.8" spans="2:8">
       <c r="B165" s="3" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>629</v>
+        <v>638</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>636</v>
+        <v>581</v>
       </c>
       <c r="F165" s="3" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="G165" s="3" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="H165" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="166" ht="100.8" spans="2:8">
+      <c r="B166" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="D166" s="3" t="s">
+        <v>638</v>
+      </c>
+      <c r="E166" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="F166" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="G166" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="H166" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="167" ht="100.8" spans="2:8">
+      <c r="B167" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="D167" s="3" t="s">
+        <v>638</v>
+      </c>
+      <c r="E167" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="F167" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="G167" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="H167" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="168" ht="57.6" spans="2:8">
+      <c r="B168" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="D168" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="E168" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="F168" s="3" t="s">
+        <v>651</v>
+      </c>
+      <c r="G168" s="3" t="s">
+        <v>651</v>
+      </c>
+      <c r="H168" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="169" ht="57.6" spans="2:8">
+      <c r="B169" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="D169" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="E169" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="F169" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="G169" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="H169" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="170" ht="57.6" spans="2:8">
+      <c r="B170" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>658</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="E170" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="F170" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="G170" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="H170" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="171" ht="57.6" spans="2:8">
+      <c r="B171" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="D171" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="E171" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="F171" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="G171" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="H171" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="172" ht="115.2" spans="2:8">
+      <c r="B172" s="3" t="s">
+        <v>667</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>668</v>
+      </c>
+      <c r="D172" s="3" t="s">
+        <v>669</v>
+      </c>
+      <c r="F172" s="3" t="s">
+        <v>670</v>
+      </c>
+      <c r="G172" s="3" t="s">
+        <v>670</v>
+      </c>
+      <c r="H172" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -8167,10 +8468,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:F52"/>
+  <dimension ref="B1:F54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -8181,566 +8482,588 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.15"/>
-    <row r="2" spans="2:4">
+    <row r="2" ht="15.15" spans="2:4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>638</v>
+        <v>671</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>639</v>
+        <v>672</v>
       </c>
     </row>
     <row r="3" ht="72" spans="2:4">
       <c r="B3" t="s">
-        <v>640</v>
+        <v>673</v>
       </c>
       <c r="C3" t="s">
-        <v>641</v>
+        <v>674</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>642</v>
+        <v>675</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" t="s">
-        <v>643</v>
+        <v>676</v>
       </c>
       <c r="C4" t="s">
-        <v>644</v>
+        <v>677</v>
       </c>
       <c r="D4" t="s">
-        <v>645</v>
+        <v>678</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" t="s">
-        <v>646</v>
+        <v>679</v>
       </c>
       <c r="C5" t="s">
-        <v>647</v>
+        <v>680</v>
       </c>
       <c r="D5" t="s">
-        <v>648</v>
+        <v>681</v>
       </c>
     </row>
     <row r="6" ht="216" spans="2:4">
       <c r="B6" t="s">
-        <v>649</v>
+        <v>682</v>
       </c>
       <c r="C6" t="s">
-        <v>650</v>
+        <v>683</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="7" ht="216" spans="2:4">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="7" ht="230.4" spans="2:4">
       <c r="B7" t="s">
-        <v>652</v>
+        <v>685</v>
       </c>
       <c r="C7" t="s">
-        <v>653</v>
+        <v>686</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="8" ht="43.2" spans="2:4">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="8" ht="57.6" spans="2:4">
       <c r="B8" t="s">
-        <v>655</v>
+        <v>688</v>
       </c>
       <c r="C8" t="s">
-        <v>656</v>
+        <v>689</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>657</v>
+        <v>690</v>
       </c>
     </row>
     <row r="9" ht="28.8" spans="2:4">
       <c r="B9" t="s">
-        <v>658</v>
+        <v>691</v>
       </c>
       <c r="C9" t="s">
-        <v>659</v>
+        <v>692</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>660</v>
+        <v>693</v>
       </c>
     </row>
     <row r="10" spans="2:4">
       <c r="B10" t="s">
-        <v>661</v>
+        <v>694</v>
       </c>
       <c r="C10" t="s">
-        <v>662</v>
+        <v>695</v>
       </c>
       <c r="D10" t="s">
-        <v>663</v>
+        <v>696</v>
       </c>
     </row>
     <row r="11" ht="100.8" spans="2:4">
       <c r="B11" t="s">
-        <v>664</v>
+        <v>697</v>
       </c>
       <c r="C11" t="s">
-        <v>665</v>
+        <v>698</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>666</v>
+        <v>699</v>
       </c>
     </row>
     <row r="12" ht="86.4" spans="2:6">
       <c r="B12" t="s">
-        <v>667</v>
+        <v>700</v>
       </c>
       <c r="C12" t="s">
-        <v>668</v>
+        <v>701</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>669</v>
+        <v>702</v>
       </c>
       <c r="F12" s="3"/>
     </row>
     <row r="13" ht="28.8" spans="2:4">
       <c r="B13" t="s">
-        <v>670</v>
+        <v>703</v>
       </c>
       <c r="C13" t="s">
-        <v>671</v>
+        <v>704</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>672</v>
+        <v>705</v>
       </c>
     </row>
     <row r="14" ht="28.8" spans="2:4">
       <c r="B14" t="s">
-        <v>673</v>
+        <v>706</v>
       </c>
       <c r="C14" t="s">
-        <v>674</v>
+        <v>707</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>675</v>
+        <v>708</v>
       </c>
     </row>
     <row r="15" spans="2:4">
       <c r="B15" t="s">
-        <v>676</v>
+        <v>709</v>
       </c>
       <c r="C15" t="s">
-        <v>677</v>
+        <v>710</v>
       </c>
       <c r="D15" t="s">
-        <v>678</v>
+        <v>711</v>
       </c>
     </row>
     <row r="16" ht="43.2" spans="2:4">
       <c r="B16" t="s">
-        <v>679</v>
+        <v>712</v>
       </c>
       <c r="C16" t="s">
-        <v>680</v>
+        <v>713</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>681</v>
+        <v>714</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>682</v>
+        <v>715</v>
       </c>
       <c r="C17" t="s">
-        <v>683</v>
+        <v>716</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>684</v>
+        <v>717</v>
       </c>
     </row>
     <row r="18" ht="28.8" spans="2:4">
       <c r="B18" t="s">
-        <v>685</v>
+        <v>718</v>
       </c>
       <c r="C18" t="s">
-        <v>686</v>
+        <v>719</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>687</v>
+        <v>720</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" t="s">
-        <v>688</v>
+        <v>721</v>
       </c>
       <c r="C19" t="s">
-        <v>689</v>
+        <v>722</v>
       </c>
       <c r="D19" t="s">
-        <v>690</v>
+        <v>723</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" t="s">
-        <v>691</v>
+        <v>724</v>
       </c>
       <c r="C20" t="s">
-        <v>692</v>
+        <v>725</v>
       </c>
       <c r="D20" t="s">
-        <v>693</v>
+        <v>726</v>
       </c>
     </row>
     <row r="21" ht="43.2" spans="2:4">
       <c r="B21" t="s">
-        <v>694</v>
+        <v>727</v>
       </c>
       <c r="C21" t="s">
-        <v>695</v>
+        <v>728</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>696</v>
+        <v>729</v>
       </c>
     </row>
     <row r="22" ht="43.2" spans="2:4">
       <c r="B22" t="s">
-        <v>697</v>
+        <v>730</v>
       </c>
       <c r="C22" t="s">
-        <v>698</v>
+        <v>731</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>699</v>
+        <v>732</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" t="s">
-        <v>700</v>
+        <v>733</v>
       </c>
       <c r="C23" t="s">
-        <v>701</v>
+        <v>734</v>
       </c>
       <c r="D23" t="s">
-        <v>702</v>
+        <v>735</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" t="s">
-        <v>703</v>
+        <v>736</v>
       </c>
       <c r="C24" t="s">
-        <v>704</v>
+        <v>737</v>
       </c>
       <c r="D24" t="s">
-        <v>705</v>
+        <v>738</v>
       </c>
     </row>
     <row r="25" ht="100.8" spans="2:4">
       <c r="B25" t="s">
-        <v>706</v>
+        <v>739</v>
       </c>
       <c r="C25" t="s">
-        <v>707</v>
+        <v>740</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>708</v>
+        <v>741</v>
       </c>
     </row>
     <row r="26" ht="100.8" spans="2:4">
       <c r="B26" t="s">
-        <v>709</v>
+        <v>742</v>
       </c>
       <c r="C26" t="s">
-        <v>710</v>
+        <v>743</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>711</v>
+        <v>744</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" t="s">
-        <v>712</v>
+        <v>745</v>
       </c>
       <c r="C27" t="s">
-        <v>713</v>
+        <v>746</v>
       </c>
       <c r="D27" t="s">
-        <v>714</v>
+        <v>747</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" t="s">
-        <v>715</v>
+        <v>748</v>
       </c>
       <c r="C28" t="s">
-        <v>716</v>
+        <v>749</v>
       </c>
       <c r="D28" t="s">
-        <v>717</v>
+        <v>750</v>
       </c>
     </row>
     <row r="29" ht="28.8" spans="2:4">
       <c r="B29" t="s">
-        <v>718</v>
+        <v>751</v>
       </c>
       <c r="C29" t="s">
-        <v>719</v>
+        <v>752</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>720</v>
+        <v>753</v>
       </c>
     </row>
     <row r="30" spans="2:4">
       <c r="B30" t="s">
-        <v>721</v>
+        <v>754</v>
       </c>
       <c r="C30" t="s">
-        <v>722</v>
+        <v>755</v>
       </c>
       <c r="D30" t="s">
-        <v>723</v>
+        <v>756</v>
       </c>
     </row>
     <row r="31" ht="86.4" spans="2:4">
       <c r="B31" t="s">
-        <v>724</v>
+        <v>757</v>
       </c>
       <c r="C31" t="s">
-        <v>725</v>
+        <v>758</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>726</v>
+        <v>759</v>
       </c>
     </row>
     <row r="32" ht="86.4" spans="2:4">
       <c r="B32" t="s">
-        <v>727</v>
+        <v>760</v>
       </c>
       <c r="C32" t="s">
-        <v>728</v>
+        <v>761</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>729</v>
+        <v>762</v>
       </c>
     </row>
     <row r="33" spans="2:4">
       <c r="B33" t="s">
-        <v>730</v>
+        <v>763</v>
       </c>
       <c r="C33" t="s">
-        <v>731</v>
+        <v>764</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>732</v>
+        <v>765</v>
       </c>
     </row>
     <row r="34" ht="28.8" spans="2:4">
       <c r="B34" t="s">
-        <v>733</v>
+        <v>766</v>
       </c>
       <c r="C34" t="s">
-        <v>734</v>
+        <v>767</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>735</v>
+        <v>768</v>
       </c>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" t="s">
-        <v>736</v>
+        <v>769</v>
       </c>
       <c r="C35" t="s">
-        <v>737</v>
+        <v>770</v>
       </c>
       <c r="D35" t="s">
-        <v>738</v>
+        <v>771</v>
       </c>
     </row>
     <row r="36" spans="2:4">
       <c r="B36" t="s">
-        <v>739</v>
+        <v>772</v>
       </c>
       <c r="C36" t="s">
-        <v>740</v>
+        <v>773</v>
       </c>
       <c r="D36" t="s">
-        <v>741</v>
+        <v>774</v>
       </c>
     </row>
     <row r="37" spans="2:4">
       <c r="B37" t="s">
-        <v>742</v>
+        <v>775</v>
       </c>
       <c r="C37" t="s">
-        <v>743</v>
+        <v>776</v>
       </c>
       <c r="D37" t="s">
-        <v>744</v>
+        <v>777</v>
       </c>
     </row>
     <row r="38" ht="187.2" spans="2:4">
       <c r="B38" t="s">
-        <v>745</v>
+        <v>778</v>
       </c>
       <c r="C38" t="s">
-        <v>746</v>
+        <v>779</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>747</v>
+        <v>780</v>
       </c>
     </row>
     <row r="39" ht="57.6" spans="2:4">
       <c r="B39" t="s">
-        <v>748</v>
+        <v>781</v>
       </c>
       <c r="C39" t="s">
-        <v>749</v>
+        <v>782</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>750</v>
+        <v>783</v>
       </c>
     </row>
     <row r="40" ht="57.6" spans="2:4">
       <c r="B40" t="s">
-        <v>751</v>
+        <v>784</v>
       </c>
       <c r="C40" t="s">
-        <v>752</v>
+        <v>785</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>753</v>
+        <v>786</v>
       </c>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" t="s">
-        <v>754</v>
+        <v>787</v>
       </c>
       <c r="C41" t="s">
-        <v>755</v>
+        <v>788</v>
       </c>
       <c r="D41" t="s">
-        <v>756</v>
+        <v>789</v>
       </c>
     </row>
     <row r="42" ht="57.6" spans="2:4">
       <c r="B42" t="s">
-        <v>757</v>
+        <v>790</v>
       </c>
       <c r="C42" t="s">
-        <v>758</v>
+        <v>791</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>759</v>
+        <v>792</v>
       </c>
     </row>
     <row r="43" spans="2:4">
       <c r="B43" t="s">
-        <v>760</v>
+        <v>793</v>
       </c>
       <c r="C43" t="s">
-        <v>761</v>
+        <v>794</v>
       </c>
       <c r="D43" t="s">
-        <v>762</v>
+        <v>795</v>
       </c>
     </row>
     <row r="44" spans="2:4">
       <c r="B44" t="s">
-        <v>763</v>
+        <v>796</v>
       </c>
       <c r="C44" t="s">
-        <v>553</v>
+        <v>562</v>
       </c>
       <c r="D44" t="s">
-        <v>764</v>
+        <v>797</v>
       </c>
     </row>
     <row r="45" ht="28.8" spans="2:4">
       <c r="B45" t="s">
-        <v>765</v>
+        <v>798</v>
       </c>
       <c r="C45" t="s">
-        <v>766</v>
+        <v>799</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>767</v>
+        <v>800</v>
       </c>
     </row>
     <row r="46" spans="2:4">
       <c r="B46" t="s">
-        <v>768</v>
+        <v>801</v>
       </c>
       <c r="C46" t="s">
-        <v>769</v>
+        <v>802</v>
       </c>
       <c r="D46" t="s">
-        <v>770</v>
+        <v>803</v>
       </c>
     </row>
     <row r="47" ht="43.2" spans="2:4">
       <c r="B47" t="s">
-        <v>771</v>
+        <v>804</v>
       </c>
       <c r="C47" t="s">
-        <v>772</v>
+        <v>805</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>773</v>
+        <v>806</v>
       </c>
     </row>
     <row r="48" ht="43.2" spans="2:4">
       <c r="B48" t="s">
-        <v>774</v>
+        <v>807</v>
       </c>
       <c r="C48" t="s">
-        <v>775</v>
+        <v>808</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>776</v>
+        <v>809</v>
       </c>
     </row>
     <row r="49" ht="43.2" spans="2:4">
       <c r="B49" t="s">
-        <v>777</v>
+        <v>810</v>
       </c>
       <c r="C49" t="s">
-        <v>778</v>
+        <v>811</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>779</v>
+        <v>812</v>
       </c>
     </row>
     <row r="50" ht="43.2" spans="2:4">
       <c r="B50" t="s">
-        <v>780</v>
+        <v>813</v>
       </c>
       <c r="C50" t="s">
-        <v>781</v>
+        <v>814</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>782</v>
+        <v>815</v>
       </c>
     </row>
     <row r="51" ht="43.2" spans="2:4">
       <c r="B51" t="s">
-        <v>783</v>
+        <v>816</v>
       </c>
       <c r="C51" t="s">
-        <v>784</v>
+        <v>817</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>785</v>
+        <v>818</v>
       </c>
     </row>
     <row r="52" ht="43.2" spans="2:4">
       <c r="B52" t="s">
-        <v>786</v>
+        <v>819</v>
       </c>
       <c r="C52" t="s">
-        <v>787</v>
+        <v>820</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>788</v>
+        <v>821</v>
+      </c>
+    </row>
+    <row r="53" ht="57.6" spans="2:4">
+      <c r="B53" t="s">
+        <v>822</v>
+      </c>
+      <c r="C53" t="s">
+        <v>823</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4">
+      <c r="B54" t="s">
+        <v>825</v>
+      </c>
+      <c r="C54" t="s">
+        <v>826</v>
+      </c>
+      <c r="D54" t="s">
+        <v>827</v>
       </c>
     </row>
   </sheetData>

</xml_diff>